<commit_message>
ThaoNX: finished Events file: SDD_GlobalConfiguration
</commit_message>
<xml_diff>
--- a/Document/Design/SDD_GlobalConfiguration.xlsx
+++ b/Document/Design/SDD_GlobalConfiguration.xlsx
@@ -1960,9 +1960,6 @@
     <t>C&amp;C13</t>
   </si>
   <si>
-    <t xml:space="preserve">Welcome </t>
-  </si>
-  <si>
     <t>System Setting</t>
   </si>
   <si>
@@ -2066,6 +2063,9 @@
   </si>
   <si>
     <t>Chuyển sang trang cấu hình site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome   </t>
   </si>
 </sst>
 </file>
@@ -2988,6 +2988,12 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3020,9 +3026,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3076,9 +3079,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3957,8 +3957,8 @@
   <dimension ref="B2:BE96"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ90" sqref="AJ90"/>
+      <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AT6" sqref="AT6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3971,285 +3971,291 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="103" t="s">
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="104" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-      <c r="V2" s="103"/>
-      <c r="W2" s="103"/>
-      <c r="X2" s="103"/>
-      <c r="Y2" s="103"/>
-      <c r="Z2" s="103"/>
-      <c r="AA2" s="103"/>
-      <c r="AB2" s="103"/>
-      <c r="AC2" s="103"/>
-      <c r="AD2" s="103"/>
-      <c r="AE2" s="103"/>
-      <c r="AF2" s="103"/>
-      <c r="AG2" s="103"/>
-      <c r="AH2" s="103"/>
-      <c r="AI2" s="103"/>
-      <c r="AJ2" s="103"/>
-      <c r="AK2" s="103"/>
-      <c r="AL2" s="103"/>
-      <c r="AM2" s="103"/>
-      <c r="AN2" s="103"/>
-      <c r="AO2" s="103"/>
-      <c r="AP2" s="103"/>
-      <c r="AQ2" s="90" t="s">
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104"/>
+      <c r="S2" s="104"/>
+      <c r="T2" s="104"/>
+      <c r="U2" s="104"/>
+      <c r="V2" s="104"/>
+      <c r="W2" s="104"/>
+      <c r="X2" s="104"/>
+      <c r="Y2" s="104"/>
+      <c r="Z2" s="104"/>
+      <c r="AA2" s="104"/>
+      <c r="AB2" s="104"/>
+      <c r="AC2" s="104"/>
+      <c r="AD2" s="104"/>
+      <c r="AE2" s="104"/>
+      <c r="AF2" s="104"/>
+      <c r="AG2" s="104"/>
+      <c r="AH2" s="104"/>
+      <c r="AI2" s="104"/>
+      <c r="AJ2" s="104"/>
+      <c r="AK2" s="104"/>
+      <c r="AL2" s="104"/>
+      <c r="AM2" s="104"/>
+      <c r="AN2" s="104"/>
+      <c r="AO2" s="104"/>
+      <c r="AP2" s="104"/>
+      <c r="AQ2" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="AR2" s="90"/>
-      <c r="AS2" s="90"/>
-      <c r="AT2" s="90"/>
-      <c r="AU2" s="90"/>
-      <c r="AV2" s="90"/>
-      <c r="AW2" s="90"/>
-      <c r="AX2" s="90" t="s">
+      <c r="AR2" s="92"/>
+      <c r="AS2" s="92"/>
+      <c r="AT2" s="92"/>
+      <c r="AU2" s="92"/>
+      <c r="AV2" s="92"/>
+      <c r="AW2" s="92"/>
+      <c r="AX2" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="AY2" s="90"/>
-      <c r="AZ2" s="90"/>
-      <c r="BA2" s="90"/>
-      <c r="BB2" s="90"/>
-      <c r="BC2" s="90"/>
-      <c r="BD2" s="90"/>
-      <c r="BE2" s="90"/>
+      <c r="AY2" s="92"/>
+      <c r="AZ2" s="92"/>
+      <c r="BA2" s="92"/>
+      <c r="BB2" s="92"/>
+      <c r="BC2" s="92"/>
+      <c r="BD2" s="92"/>
+      <c r="BE2" s="92"/>
     </row>
     <row r="3" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="103"/>
-      <c r="J3" s="103"/>
-      <c r="K3" s="103"/>
-      <c r="L3" s="103"/>
-      <c r="M3" s="103"/>
-      <c r="N3" s="103"/>
-      <c r="O3" s="103"/>
-      <c r="P3" s="103"/>
-      <c r="Q3" s="103"/>
-      <c r="R3" s="103"/>
-      <c r="S3" s="103"/>
-      <c r="T3" s="103"/>
-      <c r="U3" s="103"/>
-      <c r="V3" s="103"/>
-      <c r="W3" s="103"/>
-      <c r="X3" s="103"/>
-      <c r="Y3" s="103"/>
-      <c r="Z3" s="103"/>
-      <c r="AA3" s="103"/>
-      <c r="AB3" s="103"/>
-      <c r="AC3" s="103"/>
-      <c r="AD3" s="103"/>
-      <c r="AE3" s="103"/>
-      <c r="AF3" s="103"/>
-      <c r="AG3" s="103"/>
-      <c r="AH3" s="103"/>
-      <c r="AI3" s="103"/>
-      <c r="AJ3" s="103"/>
-      <c r="AK3" s="103"/>
-      <c r="AL3" s="103"/>
-      <c r="AM3" s="103"/>
-      <c r="AN3" s="103"/>
-      <c r="AO3" s="103"/>
-      <c r="AP3" s="103"/>
-      <c r="AQ3" s="92" t="s">
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="104"/>
+      <c r="Q3" s="104"/>
+      <c r="R3" s="104"/>
+      <c r="S3" s="104"/>
+      <c r="T3" s="104"/>
+      <c r="U3" s="104"/>
+      <c r="V3" s="104"/>
+      <c r="W3" s="104"/>
+      <c r="X3" s="104"/>
+      <c r="Y3" s="104"/>
+      <c r="Z3" s="104"/>
+      <c r="AA3" s="104"/>
+      <c r="AB3" s="104"/>
+      <c r="AC3" s="104"/>
+      <c r="AD3" s="104"/>
+      <c r="AE3" s="104"/>
+      <c r="AF3" s="104"/>
+      <c r="AG3" s="104"/>
+      <c r="AH3" s="104"/>
+      <c r="AI3" s="104"/>
+      <c r="AJ3" s="104"/>
+      <c r="AK3" s="104"/>
+      <c r="AL3" s="104"/>
+      <c r="AM3" s="104"/>
+      <c r="AN3" s="104"/>
+      <c r="AO3" s="104"/>
+      <c r="AP3" s="104"/>
+      <c r="AQ3" s="94" t="s">
         <v>108</v>
       </c>
-      <c r="AR3" s="92"/>
-      <c r="AS3" s="92"/>
-      <c r="AT3" s="92"/>
-      <c r="AU3" s="92"/>
-      <c r="AV3" s="92"/>
-      <c r="AW3" s="92"/>
-      <c r="AX3" s="93">
+      <c r="AR3" s="94"/>
+      <c r="AS3" s="94"/>
+      <c r="AT3" s="94"/>
+      <c r="AU3" s="94"/>
+      <c r="AV3" s="94"/>
+      <c r="AW3" s="94"/>
+      <c r="AX3" s="95">
         <v>40830</v>
       </c>
-      <c r="AY3" s="92"/>
-      <c r="AZ3" s="92"/>
-      <c r="BA3" s="92"/>
-      <c r="BB3" s="92"/>
-      <c r="BC3" s="92"/>
-      <c r="BD3" s="92"/>
-      <c r="BE3" s="92"/>
+      <c r="AY3" s="94"/>
+      <c r="AZ3" s="94"/>
+      <c r="BA3" s="94"/>
+      <c r="BB3" s="94"/>
+      <c r="BC3" s="94"/>
+      <c r="BD3" s="94"/>
+      <c r="BE3" s="94"/>
     </row>
     <row r="4" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B4" s="105" t="s">
+      <c r="B4" s="106" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="91"/>
-      <c r="M4" s="91"/>
-      <c r="N4" s="91"/>
-      <c r="O4" s="97" t="s">
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="100"/>
-      <c r="Q4" s="100"/>
-      <c r="R4" s="100"/>
-      <c r="S4" s="100"/>
-      <c r="T4" s="99"/>
-      <c r="U4" s="91" t="s">
+      <c r="P4" s="102"/>
+      <c r="Q4" s="102"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="101"/>
+      <c r="U4" s="93" t="s">
         <v>104</v>
       </c>
-      <c r="V4" s="91"/>
-      <c r="W4" s="91"/>
-      <c r="X4" s="91"/>
-      <c r="Y4" s="91"/>
-      <c r="Z4" s="91"/>
-      <c r="AA4" s="91"/>
-      <c r="AB4" s="91"/>
-      <c r="AC4" s="91"/>
-      <c r="AD4" s="91"/>
-      <c r="AE4" s="91"/>
-      <c r="AF4" s="91"/>
-      <c r="AG4" s="91"/>
-      <c r="AH4" s="91"/>
-      <c r="AI4" s="91"/>
-      <c r="AJ4" s="91"/>
-      <c r="AK4" s="91"/>
-      <c r="AL4" s="91"/>
-      <c r="AM4" s="91"/>
-      <c r="AN4" s="91"/>
-      <c r="AO4" s="91"/>
-      <c r="AP4" s="91"/>
-      <c r="AQ4" s="94" t="s">
+      <c r="V4" s="93"/>
+      <c r="W4" s="93"/>
+      <c r="X4" s="93"/>
+      <c r="Y4" s="93"/>
+      <c r="Z4" s="93"/>
+      <c r="AA4" s="93"/>
+      <c r="AB4" s="93"/>
+      <c r="AC4" s="93"/>
+      <c r="AD4" s="93"/>
+      <c r="AE4" s="93"/>
+      <c r="AF4" s="93"/>
+      <c r="AG4" s="93"/>
+      <c r="AH4" s="93"/>
+      <c r="AI4" s="93"/>
+      <c r="AJ4" s="93"/>
+      <c r="AK4" s="93"/>
+      <c r="AL4" s="93"/>
+      <c r="AM4" s="93"/>
+      <c r="AN4" s="93"/>
+      <c r="AO4" s="93"/>
+      <c r="AP4" s="93"/>
+      <c r="AQ4" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="AR4" s="95"/>
-      <c r="AS4" s="96"/>
-      <c r="AT4" s="104">
+      <c r="AR4" s="97"/>
+      <c r="AS4" s="98"/>
+      <c r="AT4" s="105">
         <v>40830</v>
       </c>
-      <c r="AU4" s="91"/>
-      <c r="AV4" s="91"/>
-      <c r="AW4" s="91"/>
-      <c r="AX4" s="94" t="s">
+      <c r="AU4" s="93"/>
+      <c r="AV4" s="93"/>
+      <c r="AW4" s="93"/>
+      <c r="AX4" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="AY4" s="95"/>
-      <c r="AZ4" s="95"/>
-      <c r="BA4" s="96"/>
-      <c r="BB4" s="91"/>
-      <c r="BC4" s="91"/>
-      <c r="BD4" s="91"/>
-      <c r="BE4" s="91"/>
+      <c r="AY4" s="97"/>
+      <c r="AZ4" s="97"/>
+      <c r="BA4" s="98"/>
+      <c r="BB4" s="105">
+        <v>40831</v>
+      </c>
+      <c r="BC4" s="93"/>
+      <c r="BD4" s="93"/>
+      <c r="BE4" s="93"/>
     </row>
     <row r="5" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
-      <c r="K5" s="91"/>
-      <c r="L5" s="91"/>
-      <c r="M5" s="91"/>
-      <c r="N5" s="91"/>
-      <c r="O5" s="97" t="s">
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="93"/>
+      <c r="K5" s="93"/>
+      <c r="L5" s="93"/>
+      <c r="M5" s="93"/>
+      <c r="N5" s="93"/>
+      <c r="O5" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="P5" s="100"/>
-      <c r="Q5" s="100"/>
-      <c r="R5" s="100"/>
-      <c r="S5" s="100"/>
-      <c r="T5" s="99"/>
-      <c r="U5" s="91"/>
-      <c r="V5" s="91"/>
-      <c r="W5" s="91"/>
-      <c r="X5" s="91"/>
-      <c r="Y5" s="91"/>
-      <c r="Z5" s="91"/>
-      <c r="AA5" s="91"/>
-      <c r="AB5" s="91"/>
-      <c r="AC5" s="91"/>
-      <c r="AD5" s="91"/>
-      <c r="AE5" s="91"/>
-      <c r="AF5" s="91"/>
-      <c r="AG5" s="91"/>
-      <c r="AH5" s="91"/>
-      <c r="AI5" s="91"/>
-      <c r="AJ5" s="91"/>
-      <c r="AK5" s="91"/>
-      <c r="AL5" s="91"/>
-      <c r="AM5" s="91"/>
-      <c r="AN5" s="91"/>
-      <c r="AO5" s="91"/>
-      <c r="AP5" s="91"/>
-      <c r="AQ5" s="97" t="s">
+      <c r="P5" s="102"/>
+      <c r="Q5" s="102"/>
+      <c r="R5" s="102"/>
+      <c r="S5" s="102"/>
+      <c r="T5" s="101"/>
+      <c r="U5" s="93"/>
+      <c r="V5" s="93"/>
+      <c r="W5" s="93"/>
+      <c r="X5" s="93"/>
+      <c r="Y5" s="93"/>
+      <c r="Z5" s="93"/>
+      <c r="AA5" s="93"/>
+      <c r="AB5" s="93"/>
+      <c r="AC5" s="93"/>
+      <c r="AD5" s="93"/>
+      <c r="AE5" s="93"/>
+      <c r="AF5" s="93"/>
+      <c r="AG5" s="93"/>
+      <c r="AH5" s="93"/>
+      <c r="AI5" s="93"/>
+      <c r="AJ5" s="93"/>
+      <c r="AK5" s="93"/>
+      <c r="AL5" s="93"/>
+      <c r="AM5" s="93"/>
+      <c r="AN5" s="93"/>
+      <c r="AO5" s="93"/>
+      <c r="AP5" s="93"/>
+      <c r="AQ5" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="AR5" s="98"/>
-      <c r="AS5" s="99"/>
-      <c r="AT5" s="91"/>
-      <c r="AU5" s="91"/>
-      <c r="AV5" s="91"/>
-      <c r="AW5" s="91"/>
-      <c r="AX5" s="97" t="s">
+      <c r="AR5" s="100"/>
+      <c r="AS5" s="101"/>
+      <c r="AT5" s="105">
+        <v>40834</v>
+      </c>
+      <c r="AU5" s="93"/>
+      <c r="AV5" s="93"/>
+      <c r="AW5" s="93"/>
+      <c r="AX5" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="AY5" s="100"/>
-      <c r="AZ5" s="100"/>
-      <c r="BA5" s="99"/>
-      <c r="BB5" s="91"/>
-      <c r="BC5" s="91"/>
-      <c r="BD5" s="91"/>
-      <c r="BE5" s="91"/>
+      <c r="AY5" s="102"/>
+      <c r="AZ5" s="102"/>
+      <c r="BA5" s="101"/>
+      <c r="BB5" s="105">
+        <v>40834</v>
+      </c>
+      <c r="BC5" s="93"/>
+      <c r="BD5" s="93"/>
+      <c r="BE5" s="93"/>
     </row>
     <row r="7" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="C7" s="107" t="s">
+      <c r="C7" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="107"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
-      <c r="G7" s="107"/>
-      <c r="H7" s="107"/>
+      <c r="D7" s="108"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="108"/>
+      <c r="H7" s="108"/>
     </row>
     <row r="9" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="L9" s="108" t="s">
+      <c r="L9" s="109" t="s">
         <v>110</v>
       </c>
-      <c r="M9" s="109"/>
-      <c r="N9" s="109"/>
+      <c r="M9" s="110"/>
+      <c r="N9" s="110"/>
       <c r="O9" s="50"/>
       <c r="P9" s="50"/>
       <c r="Q9" s="50"/>
@@ -4287,9 +4293,9 @@
       <c r="AW9" s="51"/>
     </row>
     <row r="10" spans="2:57" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="L10" s="110"/>
-      <c r="M10" s="111"/>
-      <c r="N10" s="111"/>
+      <c r="L10" s="111"/>
+      <c r="M10" s="112"/>
+      <c r="N10" s="112"/>
       <c r="O10" s="53"/>
       <c r="P10" s="53"/>
       <c r="Q10" s="53"/>
@@ -4335,9 +4341,9 @@
       <c r="AW10" s="60"/>
     </row>
     <row r="11" spans="2:57" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="L11" s="112"/>
-      <c r="M11" s="113"/>
-      <c r="N11" s="113"/>
+      <c r="L11" s="113"/>
+      <c r="M11" s="114"/>
+      <c r="N11" s="114"/>
       <c r="O11" s="54"/>
       <c r="P11" s="55"/>
       <c r="Q11" s="56"/>
@@ -4375,17 +4381,17 @@
       <c r="AW11" s="57"/>
     </row>
     <row r="12" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="L12" s="114" t="s">
+      <c r="L12" s="115" t="s">
         <v>114</v>
       </c>
-      <c r="M12" s="115"/>
-      <c r="N12" s="115"/>
-      <c r="O12" s="115"/>
-      <c r="P12" s="115"/>
-      <c r="Q12" s="115"/>
-      <c r="R12" s="115"/>
-      <c r="S12" s="115"/>
-      <c r="T12" s="118" t="s">
+      <c r="M12" s="116"/>
+      <c r="N12" s="116"/>
+      <c r="O12" s="116"/>
+      <c r="P12" s="116"/>
+      <c r="Q12" s="116"/>
+      <c r="R12" s="116"/>
+      <c r="S12" s="116"/>
+      <c r="T12" s="119" t="s">
         <v>115</v>
       </c>
       <c r="U12" s="84"/>
@@ -4419,14 +4425,14 @@
       <c r="AW12" s="63"/>
     </row>
     <row r="13" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="L13" s="116"/>
-      <c r="M13" s="117"/>
-      <c r="N13" s="117"/>
-      <c r="O13" s="117"/>
-      <c r="P13" s="117"/>
-      <c r="Q13" s="117"/>
-      <c r="R13" s="117"/>
-      <c r="S13" s="117"/>
+      <c r="L13" s="117"/>
+      <c r="M13" s="118"/>
+      <c r="N13" s="118"/>
+      <c r="O13" s="118"/>
+      <c r="P13" s="118"/>
+      <c r="Q13" s="118"/>
+      <c r="R13" s="118"/>
+      <c r="S13" s="118"/>
       <c r="T13" s="86"/>
       <c r="U13" s="87"/>
       <c r="V13" s="87"/>
@@ -4736,7 +4742,7 @@
       <c r="R22" s="41"/>
       <c r="S22" s="41"/>
       <c r="T22" s="61" t="s">
-        <v>138</v>
+        <v>173</v>
       </c>
       <c r="U22" s="62"/>
       <c r="V22" s="62"/>
@@ -5403,82 +5409,82 @@
       <c r="C47" s="49"/>
     </row>
     <row r="48" spans="3:56" ht="15" x14ac:dyDescent="0.2">
-      <c r="C48" s="119" t="s">
+      <c r="C48" s="120" t="s">
         <v>34</v>
       </c>
-      <c r="D48" s="101"/>
-      <c r="E48" s="101" t="s">
+      <c r="D48" s="90"/>
+      <c r="E48" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="F48" s="101"/>
-      <c r="G48" s="101"/>
-      <c r="H48" s="101"/>
-      <c r="I48" s="101"/>
-      <c r="J48" s="101"/>
-      <c r="K48" s="101"/>
-      <c r="L48" s="101"/>
-      <c r="M48" s="101"/>
-      <c r="N48" s="101" t="s">
+      <c r="F48" s="90"/>
+      <c r="G48" s="90"/>
+      <c r="H48" s="90"/>
+      <c r="I48" s="90"/>
+      <c r="J48" s="90"/>
+      <c r="K48" s="90"/>
+      <c r="L48" s="90"/>
+      <c r="M48" s="90"/>
+      <c r="N48" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="O48" s="101"/>
-      <c r="P48" s="101"/>
-      <c r="Q48" s="101"/>
-      <c r="R48" s="101" t="s">
+      <c r="O48" s="90"/>
+      <c r="P48" s="90"/>
+      <c r="Q48" s="90"/>
+      <c r="R48" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="S48" s="101"/>
-      <c r="T48" s="101"/>
-      <c r="U48" s="101" t="s">
+      <c r="S48" s="90"/>
+      <c r="T48" s="90"/>
+      <c r="U48" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="V48" s="101"/>
-      <c r="W48" s="101"/>
-      <c r="X48" s="101" t="s">
+      <c r="V48" s="90"/>
+      <c r="W48" s="90"/>
+      <c r="X48" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="Y48" s="101"/>
-      <c r="Z48" s="101"/>
-      <c r="AA48" s="101"/>
-      <c r="AB48" s="101"/>
-      <c r="AC48" s="101"/>
-      <c r="AD48" s="101"/>
-      <c r="AE48" s="101" t="s">
+      <c r="Y48" s="90"/>
+      <c r="Z48" s="90"/>
+      <c r="AA48" s="90"/>
+      <c r="AB48" s="90"/>
+      <c r="AC48" s="90"/>
+      <c r="AD48" s="90"/>
+      <c r="AE48" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="AF48" s="101"/>
-      <c r="AG48" s="101"/>
-      <c r="AH48" s="101"/>
-      <c r="AI48" s="101"/>
-      <c r="AJ48" s="101" t="s">
+      <c r="AF48" s="90"/>
+      <c r="AG48" s="90"/>
+      <c r="AH48" s="90"/>
+      <c r="AI48" s="90"/>
+      <c r="AJ48" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="AK48" s="101"/>
-      <c r="AL48" s="101"/>
-      <c r="AM48" s="101"/>
-      <c r="AN48" s="101" t="s">
+      <c r="AK48" s="90"/>
+      <c r="AL48" s="90"/>
+      <c r="AM48" s="90"/>
+      <c r="AN48" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="AO48" s="101"/>
-      <c r="AP48" s="101"/>
-      <c r="AQ48" s="101" t="s">
+      <c r="AO48" s="90"/>
+      <c r="AP48" s="90"/>
+      <c r="AQ48" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="AR48" s="101"/>
-      <c r="AS48" s="101"/>
-      <c r="AT48" s="101"/>
-      <c r="AU48" s="101"/>
-      <c r="AV48" s="101"/>
-      <c r="AW48" s="101" t="s">
+      <c r="AR48" s="90"/>
+      <c r="AS48" s="90"/>
+      <c r="AT48" s="90"/>
+      <c r="AU48" s="90"/>
+      <c r="AV48" s="90"/>
+      <c r="AW48" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="AX48" s="101"/>
-      <c r="AY48" s="101"/>
-      <c r="AZ48" s="101"/>
-      <c r="BA48" s="101"/>
-      <c r="BB48" s="101"/>
-      <c r="BC48" s="101"/>
-      <c r="BD48" s="120"/>
+      <c r="AX48" s="90"/>
+      <c r="AY48" s="90"/>
+      <c r="AZ48" s="90"/>
+      <c r="BA48" s="90"/>
+      <c r="BB48" s="90"/>
+      <c r="BC48" s="90"/>
+      <c r="BD48" s="91"/>
     </row>
     <row r="49" spans="3:56" x14ac:dyDescent="0.2">
       <c r="C49" s="30"/>
@@ -5867,7 +5873,7 @@
       <c r="F54" s="35"/>
       <c r="G54" s="35"/>
       <c r="H54" s="35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I54" s="35"/>
       <c r="J54" s="35"/>
@@ -5894,7 +5900,7 @@
       <c r="Y54" s="32"/>
       <c r="Z54" s="32"/>
       <c r="AA54" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AB54" s="35"/>
       <c r="AC54" s="35"/>
@@ -5927,7 +5933,7 @@
       <c r="AV54" s="35"/>
       <c r="AW54" s="36"/>
       <c r="AX54" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AY54" s="35"/>
       <c r="AZ54" s="35"/>
@@ -6122,7 +6128,7 @@
       <c r="Y57" s="32"/>
       <c r="Z57" s="32"/>
       <c r="AA57" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AB57" s="35"/>
       <c r="AC57" s="35"/>
@@ -6198,7 +6204,7 @@
       <c r="Y58" s="32"/>
       <c r="Z58" s="32"/>
       <c r="AA58" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AB58" s="35"/>
       <c r="AC58" s="35"/>
@@ -6274,7 +6280,7 @@
       <c r="Y59" s="32"/>
       <c r="Z59" s="32"/>
       <c r="AA59" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AB59" s="35"/>
       <c r="AC59" s="35"/>
@@ -6607,7 +6613,7 @@
       <c r="Q66" s="34"/>
       <c r="R66" s="31"/>
       <c r="S66" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T66" s="31"/>
       <c r="U66" s="31"/>
@@ -6673,7 +6679,7 @@
       <c r="Q67" s="37"/>
       <c r="R67" s="35"/>
       <c r="S67" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T67" s="35"/>
       <c r="U67" s="35"/>
@@ -6739,7 +6745,7 @@
       <c r="Q68" s="37"/>
       <c r="R68" s="35"/>
       <c r="S68" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T68" s="35"/>
       <c r="U68" s="35"/>
@@ -6805,7 +6811,7 @@
       <c r="Q69" s="37"/>
       <c r="R69" s="35"/>
       <c r="S69" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T69" s="35"/>
       <c r="U69" s="35"/>
@@ -6871,7 +6877,7 @@
       <c r="Q70" s="37"/>
       <c r="R70" s="35"/>
       <c r="S70" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T70" s="35"/>
       <c r="U70" s="35"/>
@@ -7567,7 +7573,7 @@
       <c r="R85" s="31"/>
       <c r="S85" s="31"/>
       <c r="T85" s="31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U85" s="31"/>
       <c r="V85" s="31"/>
@@ -7585,7 +7591,7 @@
       <c r="AH85" s="31"/>
       <c r="AI85" s="31"/>
       <c r="AJ85" s="31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AK85" s="31"/>
       <c r="AL85" s="31"/>
@@ -7629,7 +7635,7 @@
       <c r="R86" s="35"/>
       <c r="S86" s="35"/>
       <c r="T86" s="31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U86" s="35"/>
       <c r="V86" s="35"/>
@@ -7647,7 +7653,7 @@
       <c r="AH86" s="35"/>
       <c r="AI86" s="35"/>
       <c r="AJ86" s="35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AK86" s="35"/>
       <c r="AL86" s="35"/>
@@ -7691,7 +7697,7 @@
       <c r="R87" s="35"/>
       <c r="S87" s="35"/>
       <c r="T87" s="31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U87" s="35"/>
       <c r="V87" s="35"/>
@@ -7709,7 +7715,7 @@
       <c r="AH87" s="35"/>
       <c r="AI87" s="35"/>
       <c r="AJ87" s="35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AK87" s="35"/>
       <c r="AL87" s="35"/>
@@ -7753,7 +7759,7 @@
       <c r="R88" s="35"/>
       <c r="S88" s="35"/>
       <c r="T88" s="31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U88" s="35"/>
       <c r="V88" s="35"/>
@@ -7771,7 +7777,7 @@
       <c r="AH88" s="35"/>
       <c r="AI88" s="35"/>
       <c r="AJ88" s="35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AK88" s="35"/>
       <c r="AL88" s="35"/>
@@ -7815,7 +7821,7 @@
       <c r="R89" s="35"/>
       <c r="S89" s="35"/>
       <c r="T89" s="31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U89" s="35"/>
       <c r="V89" s="35"/>
@@ -7833,7 +7839,7 @@
       <c r="AH89" s="35"/>
       <c r="AI89" s="35"/>
       <c r="AJ89" s="35" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AK89" s="35"/>
       <c r="AL89" s="35"/>
@@ -8332,285 +8338,285 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="103" t="s">
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="104" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-      <c r="V2" s="103"/>
-      <c r="W2" s="103"/>
-      <c r="X2" s="103"/>
-      <c r="Y2" s="103"/>
-      <c r="Z2" s="103"/>
-      <c r="AA2" s="103"/>
-      <c r="AB2" s="103"/>
-      <c r="AC2" s="103"/>
-      <c r="AD2" s="103"/>
-      <c r="AE2" s="103"/>
-      <c r="AF2" s="103"/>
-      <c r="AG2" s="103"/>
-      <c r="AH2" s="103"/>
-      <c r="AI2" s="103"/>
-      <c r="AJ2" s="103"/>
-      <c r="AK2" s="103"/>
-      <c r="AL2" s="103"/>
-      <c r="AM2" s="103"/>
-      <c r="AN2" s="103"/>
-      <c r="AO2" s="103"/>
-      <c r="AP2" s="103"/>
-      <c r="AQ2" s="90" t="s">
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104"/>
+      <c r="S2" s="104"/>
+      <c r="T2" s="104"/>
+      <c r="U2" s="104"/>
+      <c r="V2" s="104"/>
+      <c r="W2" s="104"/>
+      <c r="X2" s="104"/>
+      <c r="Y2" s="104"/>
+      <c r="Z2" s="104"/>
+      <c r="AA2" s="104"/>
+      <c r="AB2" s="104"/>
+      <c r="AC2" s="104"/>
+      <c r="AD2" s="104"/>
+      <c r="AE2" s="104"/>
+      <c r="AF2" s="104"/>
+      <c r="AG2" s="104"/>
+      <c r="AH2" s="104"/>
+      <c r="AI2" s="104"/>
+      <c r="AJ2" s="104"/>
+      <c r="AK2" s="104"/>
+      <c r="AL2" s="104"/>
+      <c r="AM2" s="104"/>
+      <c r="AN2" s="104"/>
+      <c r="AO2" s="104"/>
+      <c r="AP2" s="104"/>
+      <c r="AQ2" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="AR2" s="90"/>
-      <c r="AS2" s="90"/>
-      <c r="AT2" s="90"/>
-      <c r="AU2" s="90"/>
-      <c r="AV2" s="90"/>
-      <c r="AW2" s="90"/>
-      <c r="AX2" s="90" t="s">
+      <c r="AR2" s="92"/>
+      <c r="AS2" s="92"/>
+      <c r="AT2" s="92"/>
+      <c r="AU2" s="92"/>
+      <c r="AV2" s="92"/>
+      <c r="AW2" s="92"/>
+      <c r="AX2" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="AY2" s="90"/>
-      <c r="AZ2" s="90"/>
-      <c r="BA2" s="90"/>
-      <c r="BB2" s="90"/>
-      <c r="BC2" s="90"/>
-      <c r="BD2" s="90"/>
-      <c r="BE2" s="90"/>
+      <c r="AY2" s="92"/>
+      <c r="AZ2" s="92"/>
+      <c r="BA2" s="92"/>
+      <c r="BB2" s="92"/>
+      <c r="BC2" s="92"/>
+      <c r="BD2" s="92"/>
+      <c r="BE2" s="92"/>
     </row>
     <row r="3" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="103"/>
-      <c r="J3" s="103"/>
-      <c r="K3" s="103"/>
-      <c r="L3" s="103"/>
-      <c r="M3" s="103"/>
-      <c r="N3" s="103"/>
-      <c r="O3" s="103"/>
-      <c r="P3" s="103"/>
-      <c r="Q3" s="103"/>
-      <c r="R3" s="103"/>
-      <c r="S3" s="103"/>
-      <c r="T3" s="103"/>
-      <c r="U3" s="103"/>
-      <c r="V3" s="103"/>
-      <c r="W3" s="103"/>
-      <c r="X3" s="103"/>
-      <c r="Y3" s="103"/>
-      <c r="Z3" s="103"/>
-      <c r="AA3" s="103"/>
-      <c r="AB3" s="103"/>
-      <c r="AC3" s="103"/>
-      <c r="AD3" s="103"/>
-      <c r="AE3" s="103"/>
-      <c r="AF3" s="103"/>
-      <c r="AG3" s="103"/>
-      <c r="AH3" s="103"/>
-      <c r="AI3" s="103"/>
-      <c r="AJ3" s="103"/>
-      <c r="AK3" s="103"/>
-      <c r="AL3" s="103"/>
-      <c r="AM3" s="103"/>
-      <c r="AN3" s="103"/>
-      <c r="AO3" s="103"/>
-      <c r="AP3" s="103"/>
-      <c r="AQ3" s="92" t="s">
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="104"/>
+      <c r="Q3" s="104"/>
+      <c r="R3" s="104"/>
+      <c r="S3" s="104"/>
+      <c r="T3" s="104"/>
+      <c r="U3" s="104"/>
+      <c r="V3" s="104"/>
+      <c r="W3" s="104"/>
+      <c r="X3" s="104"/>
+      <c r="Y3" s="104"/>
+      <c r="Z3" s="104"/>
+      <c r="AA3" s="104"/>
+      <c r="AB3" s="104"/>
+      <c r="AC3" s="104"/>
+      <c r="AD3" s="104"/>
+      <c r="AE3" s="104"/>
+      <c r="AF3" s="104"/>
+      <c r="AG3" s="104"/>
+      <c r="AH3" s="104"/>
+      <c r="AI3" s="104"/>
+      <c r="AJ3" s="104"/>
+      <c r="AK3" s="104"/>
+      <c r="AL3" s="104"/>
+      <c r="AM3" s="104"/>
+      <c r="AN3" s="104"/>
+      <c r="AO3" s="104"/>
+      <c r="AP3" s="104"/>
+      <c r="AQ3" s="94" t="s">
         <v>108</v>
       </c>
-      <c r="AR3" s="92"/>
-      <c r="AS3" s="92"/>
-      <c r="AT3" s="92"/>
-      <c r="AU3" s="92"/>
-      <c r="AV3" s="92"/>
-      <c r="AW3" s="92"/>
-      <c r="AX3" s="93">
+      <c r="AR3" s="94"/>
+      <c r="AS3" s="94"/>
+      <c r="AT3" s="94"/>
+      <c r="AU3" s="94"/>
+      <c r="AV3" s="94"/>
+      <c r="AW3" s="94"/>
+      <c r="AX3" s="95">
         <v>40830</v>
       </c>
-      <c r="AY3" s="92"/>
-      <c r="AZ3" s="92"/>
-      <c r="BA3" s="92"/>
-      <c r="BB3" s="92"/>
-      <c r="BC3" s="92"/>
-      <c r="BD3" s="92"/>
-      <c r="BE3" s="92"/>
+      <c r="AY3" s="94"/>
+      <c r="AZ3" s="94"/>
+      <c r="BA3" s="94"/>
+      <c r="BB3" s="94"/>
+      <c r="BC3" s="94"/>
+      <c r="BD3" s="94"/>
+      <c r="BE3" s="94"/>
     </row>
     <row r="4" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B4" s="105" t="s">
+      <c r="B4" s="106" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="91"/>
-      <c r="M4" s="91"/>
-      <c r="N4" s="91"/>
-      <c r="O4" s="97" t="s">
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="100"/>
-      <c r="Q4" s="100"/>
-      <c r="R4" s="100"/>
-      <c r="S4" s="100"/>
-      <c r="T4" s="99"/>
-      <c r="U4" s="91" t="s">
+      <c r="P4" s="102"/>
+      <c r="Q4" s="102"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="101"/>
+      <c r="U4" s="93" t="s">
         <v>104</v>
       </c>
-      <c r="V4" s="91"/>
-      <c r="W4" s="91"/>
-      <c r="X4" s="91"/>
-      <c r="Y4" s="91"/>
-      <c r="Z4" s="91"/>
-      <c r="AA4" s="91"/>
-      <c r="AB4" s="91"/>
-      <c r="AC4" s="91"/>
-      <c r="AD4" s="91"/>
-      <c r="AE4" s="91"/>
-      <c r="AF4" s="91"/>
-      <c r="AG4" s="91"/>
-      <c r="AH4" s="91"/>
-      <c r="AI4" s="91"/>
-      <c r="AJ4" s="91"/>
-      <c r="AK4" s="91"/>
-      <c r="AL4" s="91"/>
-      <c r="AM4" s="91"/>
-      <c r="AN4" s="91"/>
-      <c r="AO4" s="91"/>
-      <c r="AP4" s="91"/>
-      <c r="AQ4" s="94" t="s">
+      <c r="V4" s="93"/>
+      <c r="W4" s="93"/>
+      <c r="X4" s="93"/>
+      <c r="Y4" s="93"/>
+      <c r="Z4" s="93"/>
+      <c r="AA4" s="93"/>
+      <c r="AB4" s="93"/>
+      <c r="AC4" s="93"/>
+      <c r="AD4" s="93"/>
+      <c r="AE4" s="93"/>
+      <c r="AF4" s="93"/>
+      <c r="AG4" s="93"/>
+      <c r="AH4" s="93"/>
+      <c r="AI4" s="93"/>
+      <c r="AJ4" s="93"/>
+      <c r="AK4" s="93"/>
+      <c r="AL4" s="93"/>
+      <c r="AM4" s="93"/>
+      <c r="AN4" s="93"/>
+      <c r="AO4" s="93"/>
+      <c r="AP4" s="93"/>
+      <c r="AQ4" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="AR4" s="95"/>
-      <c r="AS4" s="96"/>
-      <c r="AT4" s="104">
+      <c r="AR4" s="97"/>
+      <c r="AS4" s="98"/>
+      <c r="AT4" s="105">
         <v>40830</v>
       </c>
-      <c r="AU4" s="91"/>
-      <c r="AV4" s="91"/>
-      <c r="AW4" s="91"/>
-      <c r="AX4" s="94" t="s">
+      <c r="AU4" s="93"/>
+      <c r="AV4" s="93"/>
+      <c r="AW4" s="93"/>
+      <c r="AX4" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="AY4" s="95"/>
-      <c r="AZ4" s="95"/>
-      <c r="BA4" s="96"/>
-      <c r="BB4" s="91"/>
-      <c r="BC4" s="91"/>
-      <c r="BD4" s="91"/>
-      <c r="BE4" s="91"/>
+      <c r="AY4" s="97"/>
+      <c r="AZ4" s="97"/>
+      <c r="BA4" s="98"/>
+      <c r="BB4" s="93"/>
+      <c r="BC4" s="93"/>
+      <c r="BD4" s="93"/>
+      <c r="BE4" s="93"/>
     </row>
     <row r="5" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
-      <c r="K5" s="91"/>
-      <c r="L5" s="91"/>
-      <c r="M5" s="91"/>
-      <c r="N5" s="91"/>
-      <c r="O5" s="97" t="s">
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="93"/>
+      <c r="K5" s="93"/>
+      <c r="L5" s="93"/>
+      <c r="M5" s="93"/>
+      <c r="N5" s="93"/>
+      <c r="O5" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="P5" s="100"/>
-      <c r="Q5" s="100"/>
-      <c r="R5" s="100"/>
-      <c r="S5" s="100"/>
-      <c r="T5" s="99"/>
-      <c r="U5" s="91"/>
-      <c r="V5" s="91"/>
-      <c r="W5" s="91"/>
-      <c r="X5" s="91"/>
-      <c r="Y5" s="91"/>
-      <c r="Z5" s="91"/>
-      <c r="AA5" s="91"/>
-      <c r="AB5" s="91"/>
-      <c r="AC5" s="91"/>
-      <c r="AD5" s="91"/>
-      <c r="AE5" s="91"/>
-      <c r="AF5" s="91"/>
-      <c r="AG5" s="91"/>
-      <c r="AH5" s="91"/>
-      <c r="AI5" s="91"/>
-      <c r="AJ5" s="91"/>
-      <c r="AK5" s="91"/>
-      <c r="AL5" s="91"/>
-      <c r="AM5" s="91"/>
-      <c r="AN5" s="91"/>
-      <c r="AO5" s="91"/>
-      <c r="AP5" s="91"/>
-      <c r="AQ5" s="97" t="s">
+      <c r="P5" s="102"/>
+      <c r="Q5" s="102"/>
+      <c r="R5" s="102"/>
+      <c r="S5" s="102"/>
+      <c r="T5" s="101"/>
+      <c r="U5" s="93"/>
+      <c r="V5" s="93"/>
+      <c r="W5" s="93"/>
+      <c r="X5" s="93"/>
+      <c r="Y5" s="93"/>
+      <c r="Z5" s="93"/>
+      <c r="AA5" s="93"/>
+      <c r="AB5" s="93"/>
+      <c r="AC5" s="93"/>
+      <c r="AD5" s="93"/>
+      <c r="AE5" s="93"/>
+      <c r="AF5" s="93"/>
+      <c r="AG5" s="93"/>
+      <c r="AH5" s="93"/>
+      <c r="AI5" s="93"/>
+      <c r="AJ5" s="93"/>
+      <c r="AK5" s="93"/>
+      <c r="AL5" s="93"/>
+      <c r="AM5" s="93"/>
+      <c r="AN5" s="93"/>
+      <c r="AO5" s="93"/>
+      <c r="AP5" s="93"/>
+      <c r="AQ5" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="AR5" s="98"/>
-      <c r="AS5" s="99"/>
-      <c r="AT5" s="91"/>
-      <c r="AU5" s="91"/>
-      <c r="AV5" s="91"/>
-      <c r="AW5" s="91"/>
-      <c r="AX5" s="97" t="s">
+      <c r="AR5" s="100"/>
+      <c r="AS5" s="101"/>
+      <c r="AT5" s="93"/>
+      <c r="AU5" s="93"/>
+      <c r="AV5" s="93"/>
+      <c r="AW5" s="93"/>
+      <c r="AX5" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="AY5" s="100"/>
-      <c r="AZ5" s="100"/>
-      <c r="BA5" s="99"/>
-      <c r="BB5" s="91"/>
-      <c r="BC5" s="91"/>
-      <c r="BD5" s="91"/>
-      <c r="BE5" s="91"/>
+      <c r="AY5" s="102"/>
+      <c r="AZ5" s="102"/>
+      <c r="BA5" s="101"/>
+      <c r="BB5" s="93"/>
+      <c r="BC5" s="93"/>
+      <c r="BD5" s="93"/>
+      <c r="BE5" s="93"/>
     </row>
     <row r="7" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="C7" s="107" t="s">
+      <c r="C7" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="107"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
-      <c r="G7" s="107"/>
-      <c r="H7" s="107"/>
+      <c r="D7" s="108"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="108"/>
+      <c r="H7" s="108"/>
     </row>
     <row r="9" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="L9" s="108" t="s">
+      <c r="L9" s="109" t="s">
         <v>110</v>
       </c>
-      <c r="M9" s="109"/>
-      <c r="N9" s="109"/>
+      <c r="M9" s="110"/>
+      <c r="N9" s="110"/>
       <c r="O9" s="50"/>
       <c r="P9" s="50"/>
       <c r="Q9" s="50"/>
@@ -8648,9 +8654,9 @@
       <c r="AW9" s="51"/>
     </row>
     <row r="10" spans="2:57" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="L10" s="110"/>
-      <c r="M10" s="111"/>
-      <c r="N10" s="111"/>
+      <c r="L10" s="111"/>
+      <c r="M10" s="112"/>
+      <c r="N10" s="112"/>
       <c r="O10" s="53"/>
       <c r="P10" s="53"/>
       <c r="Q10" s="53"/>
@@ -8696,9 +8702,9 @@
       <c r="AW10" s="60"/>
     </row>
     <row r="11" spans="2:57" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="L11" s="112"/>
-      <c r="M11" s="113"/>
-      <c r="N11" s="113"/>
+      <c r="L11" s="113"/>
+      <c r="M11" s="114"/>
+      <c r="N11" s="114"/>
       <c r="O11" s="54"/>
       <c r="P11" s="55"/>
       <c r="Q11" s="56"/>
@@ -8736,7 +8742,7 @@
       <c r="AW11" s="57"/>
     </row>
     <row r="12" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="L12" s="118" t="s">
+      <c r="L12" s="119" t="s">
         <v>114</v>
       </c>
       <c r="M12" s="84"/>
@@ -8746,14 +8752,14 @@
       <c r="Q12" s="84"/>
       <c r="R12" s="84"/>
       <c r="S12" s="84"/>
-      <c r="T12" s="114" t="s">
+      <c r="T12" s="115" t="s">
         <v>115</v>
       </c>
-      <c r="U12" s="115"/>
-      <c r="V12" s="115"/>
-      <c r="W12" s="115"/>
-      <c r="X12" s="115"/>
-      <c r="Y12" s="115"/>
+      <c r="U12" s="116"/>
+      <c r="V12" s="116"/>
+      <c r="W12" s="116"/>
+      <c r="X12" s="116"/>
+      <c r="Y12" s="116"/>
       <c r="Z12" s="77"/>
       <c r="AA12" s="62"/>
       <c r="AB12" s="62"/>
@@ -8788,12 +8794,12 @@
       <c r="Q13" s="87"/>
       <c r="R13" s="87"/>
       <c r="S13" s="87"/>
-      <c r="T13" s="116"/>
-      <c r="U13" s="117"/>
-      <c r="V13" s="117"/>
-      <c r="W13" s="117"/>
-      <c r="X13" s="117"/>
-      <c r="Y13" s="117"/>
+      <c r="T13" s="117"/>
+      <c r="U13" s="118"/>
+      <c r="V13" s="118"/>
+      <c r="W13" s="118"/>
+      <c r="X13" s="118"/>
+      <c r="Y13" s="118"/>
       <c r="Z13" s="78"/>
       <c r="AA13" s="65"/>
       <c r="AB13" s="65"/>
@@ -8821,7 +8827,7 @@
     </row>
     <row r="15" spans="2:57" x14ac:dyDescent="0.2">
       <c r="L15" s="83" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M15" s="84"/>
       <c r="N15" s="84"/>
@@ -8985,7 +8991,7 @@
       <c r="L19" s="44"/>
       <c r="M19" s="41"/>
       <c r="N19" s="41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O19" s="41"/>
       <c r="P19" s="41"/>
@@ -8995,7 +9001,7 @@
       <c r="T19" s="74"/>
       <c r="U19" s="74"/>
       <c r="V19" s="74" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="W19" s="74"/>
       <c r="X19" s="74"/>
@@ -9069,7 +9075,7 @@
       <c r="L21" s="44"/>
       <c r="M21" s="41"/>
       <c r="N21" s="41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O21" s="41"/>
       <c r="P21" s="41"/>
@@ -9079,7 +9085,7 @@
       <c r="T21" s="74"/>
       <c r="U21" s="74"/>
       <c r="V21" s="74" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="W21" s="74"/>
       <c r="X21" s="74"/>
@@ -9153,7 +9159,7 @@
       <c r="L23" s="44"/>
       <c r="M23" s="41"/>
       <c r="N23" s="41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O23" s="41"/>
       <c r="P23" s="41"/>
@@ -9163,7 +9169,7 @@
       <c r="T23" s="74"/>
       <c r="U23" s="74"/>
       <c r="V23" s="74" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="W23" s="74"/>
       <c r="X23" s="74"/>
@@ -9237,7 +9243,7 @@
       <c r="L25" s="44"/>
       <c r="M25" s="41"/>
       <c r="N25" s="41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O25" s="41"/>
       <c r="P25" s="41"/>
@@ -9247,7 +9253,7 @@
       <c r="T25" s="74"/>
       <c r="U25" s="74"/>
       <c r="V25" s="74" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="W25" s="74"/>
       <c r="X25" s="74"/>
@@ -9321,7 +9327,7 @@
       <c r="L27" s="44"/>
       <c r="M27" s="41"/>
       <c r="N27" s="41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O27" s="41"/>
       <c r="P27" s="41"/>
@@ -9331,7 +9337,7 @@
       <c r="T27" s="74"/>
       <c r="U27" s="74"/>
       <c r="V27" s="74" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="W27" s="74"/>
       <c r="X27" s="74"/>
@@ -9445,7 +9451,7 @@
       <c r="L30" s="44"/>
       <c r="M30" s="41"/>
       <c r="N30" s="41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O30" s="41"/>
       <c r="P30" s="41"/>
@@ -9455,7 +9461,7 @@
         <v>128</v>
       </c>
       <c r="T30" s="41" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="U30" s="41"/>
       <c r="V30" s="41"/>
@@ -9535,7 +9541,7 @@
       <c r="L32" s="44"/>
       <c r="M32" s="41"/>
       <c r="N32" s="41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O32" s="41"/>
       <c r="P32" s="41"/>
@@ -9545,7 +9551,7 @@
       <c r="T32" s="74"/>
       <c r="U32" s="74"/>
       <c r="V32" s="74" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="W32" s="74"/>
       <c r="X32" s="74"/>
@@ -9619,7 +9625,7 @@
       <c r="L34" s="44"/>
       <c r="M34" s="41"/>
       <c r="N34" s="41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O34" s="41"/>
       <c r="P34" s="41"/>
@@ -9701,7 +9707,7 @@
       <c r="L36" s="44"/>
       <c r="M36" s="41"/>
       <c r="N36" s="41" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O36" s="41"/>
       <c r="P36" s="41"/>
@@ -9912,82 +9918,82 @@
       <c r="C42" s="29"/>
     </row>
     <row r="43" spans="3:56" ht="15" x14ac:dyDescent="0.2">
-      <c r="C43" s="119" t="s">
+      <c r="C43" s="120" t="s">
         <v>34</v>
       </c>
-      <c r="D43" s="101"/>
-      <c r="E43" s="101" t="s">
+      <c r="D43" s="90"/>
+      <c r="E43" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="F43" s="101"/>
-      <c r="G43" s="101"/>
-      <c r="H43" s="101"/>
-      <c r="I43" s="101"/>
-      <c r="J43" s="101"/>
-      <c r="K43" s="101"/>
-      <c r="L43" s="101"/>
-      <c r="M43" s="101"/>
-      <c r="N43" s="101" t="s">
+      <c r="F43" s="90"/>
+      <c r="G43" s="90"/>
+      <c r="H43" s="90"/>
+      <c r="I43" s="90"/>
+      <c r="J43" s="90"/>
+      <c r="K43" s="90"/>
+      <c r="L43" s="90"/>
+      <c r="M43" s="90"/>
+      <c r="N43" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="O43" s="101"/>
-      <c r="P43" s="101"/>
-      <c r="Q43" s="101"/>
-      <c r="R43" s="101" t="s">
+      <c r="O43" s="90"/>
+      <c r="P43" s="90"/>
+      <c r="Q43" s="90"/>
+      <c r="R43" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="S43" s="101"/>
-      <c r="T43" s="101"/>
-      <c r="U43" s="101" t="s">
+      <c r="S43" s="90"/>
+      <c r="T43" s="90"/>
+      <c r="U43" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="V43" s="101"/>
-      <c r="W43" s="101"/>
-      <c r="X43" s="101" t="s">
+      <c r="V43" s="90"/>
+      <c r="W43" s="90"/>
+      <c r="X43" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="Y43" s="101"/>
-      <c r="Z43" s="101"/>
-      <c r="AA43" s="101"/>
-      <c r="AB43" s="101"/>
-      <c r="AC43" s="101"/>
-      <c r="AD43" s="101"/>
-      <c r="AE43" s="101" t="s">
+      <c r="Y43" s="90"/>
+      <c r="Z43" s="90"/>
+      <c r="AA43" s="90"/>
+      <c r="AB43" s="90"/>
+      <c r="AC43" s="90"/>
+      <c r="AD43" s="90"/>
+      <c r="AE43" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="AF43" s="101"/>
-      <c r="AG43" s="101"/>
-      <c r="AH43" s="101"/>
-      <c r="AI43" s="101"/>
-      <c r="AJ43" s="101" t="s">
+      <c r="AF43" s="90"/>
+      <c r="AG43" s="90"/>
+      <c r="AH43" s="90"/>
+      <c r="AI43" s="90"/>
+      <c r="AJ43" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="AK43" s="101"/>
-      <c r="AL43" s="101"/>
-      <c r="AM43" s="101"/>
-      <c r="AN43" s="101" t="s">
+      <c r="AK43" s="90"/>
+      <c r="AL43" s="90"/>
+      <c r="AM43" s="90"/>
+      <c r="AN43" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="AO43" s="101"/>
-      <c r="AP43" s="101"/>
-      <c r="AQ43" s="101" t="s">
+      <c r="AO43" s="90"/>
+      <c r="AP43" s="90"/>
+      <c r="AQ43" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="AR43" s="101"/>
-      <c r="AS43" s="101"/>
-      <c r="AT43" s="101"/>
-      <c r="AU43" s="101"/>
-      <c r="AV43" s="101"/>
-      <c r="AW43" s="101" t="s">
+      <c r="AR43" s="90"/>
+      <c r="AS43" s="90"/>
+      <c r="AT43" s="90"/>
+      <c r="AU43" s="90"/>
+      <c r="AV43" s="90"/>
+      <c r="AW43" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="AX43" s="101"/>
-      <c r="AY43" s="101"/>
-      <c r="AZ43" s="101"/>
-      <c r="BA43" s="101"/>
-      <c r="BB43" s="101"/>
-      <c r="BC43" s="101"/>
-      <c r="BD43" s="120"/>
+      <c r="AX43" s="90"/>
+      <c r="AY43" s="90"/>
+      <c r="AZ43" s="90"/>
+      <c r="BA43" s="90"/>
+      <c r="BB43" s="90"/>
+      <c r="BC43" s="90"/>
+      <c r="BD43" s="91"/>
     </row>
     <row r="44" spans="3:56" x14ac:dyDescent="0.2">
       <c r="C44" s="30"/>
@@ -11420,7 +11426,7 @@
       <c r="Q65" s="34"/>
       <c r="R65" s="31"/>
       <c r="S65" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T65" s="31"/>
       <c r="U65" s="31"/>
@@ -11484,7 +11490,7 @@
       <c r="Q66" s="37"/>
       <c r="R66" s="35"/>
       <c r="S66" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T66" s="31"/>
       <c r="U66" s="31"/>
@@ -11548,7 +11554,7 @@
       <c r="Q67" s="37"/>
       <c r="R67" s="35"/>
       <c r="S67" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T67" s="31"/>
       <c r="U67" s="31"/>
@@ -11612,7 +11618,7 @@
       <c r="Q68" s="37"/>
       <c r="R68" s="35"/>
       <c r="S68" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T68" s="31"/>
       <c r="U68" s="31"/>
@@ -11676,7 +11682,7 @@
       <c r="Q69" s="37"/>
       <c r="R69" s="35"/>
       <c r="S69" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T69" s="31"/>
       <c r="U69" s="31"/>
@@ -11740,7 +11746,7 @@
       <c r="Q70" s="37"/>
       <c r="R70" s="35"/>
       <c r="S70" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T70" s="31"/>
       <c r="U70" s="31"/>
@@ -11804,7 +11810,7 @@
       <c r="Q71" s="37"/>
       <c r="R71" s="35"/>
       <c r="S71" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T71" s="31"/>
       <c r="U71" s="31"/>
@@ -11868,7 +11874,7 @@
       <c r="Q72" s="37"/>
       <c r="R72" s="35"/>
       <c r="S72" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T72" s="31"/>
       <c r="U72" s="31"/>
@@ -11932,7 +11938,7 @@
       <c r="Q73" s="37"/>
       <c r="R73" s="35"/>
       <c r="S73" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T73" s="31"/>
       <c r="U73" s="31"/>
@@ -11996,7 +12002,7 @@
       <c r="Q74" s="37"/>
       <c r="R74" s="35"/>
       <c r="S74" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T74" s="31"/>
       <c r="U74" s="31"/>
@@ -12060,7 +12066,7 @@
       <c r="Q75" s="37"/>
       <c r="R75" s="35"/>
       <c r="S75" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T75" s="31"/>
       <c r="U75" s="31"/>
@@ -12418,7 +12424,7 @@
       <c r="R84" s="31"/>
       <c r="S84" s="31"/>
       <c r="T84" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="U84" s="31"/>
       <c r="V84" s="31"/>
@@ -12437,7 +12443,7 @@
       <c r="AI84" s="31"/>
       <c r="AJ84" s="31"/>
       <c r="AK84" s="31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AL84" s="31"/>
       <c r="AM84" s="31"/>
@@ -12480,7 +12486,7 @@
       <c r="R85" s="35"/>
       <c r="S85" s="35"/>
       <c r="T85" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="U85" s="35"/>
       <c r="V85" s="35"/>
@@ -12499,7 +12505,7 @@
       <c r="AI85" s="35"/>
       <c r="AJ85" s="35"/>
       <c r="AK85" s="35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AL85" s="35"/>
       <c r="AM85" s="35"/>
@@ -12542,7 +12548,7 @@
       <c r="R86" s="35"/>
       <c r="S86" s="35"/>
       <c r="T86" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="U86" s="35"/>
       <c r="V86" s="35"/>
@@ -12561,7 +12567,7 @@
       <c r="AI86" s="35"/>
       <c r="AJ86" s="35"/>
       <c r="AK86" s="35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AL86" s="35"/>
       <c r="AM86" s="35"/>
@@ -12604,7 +12610,7 @@
       <c r="R87" s="35"/>
       <c r="S87" s="35"/>
       <c r="T87" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="U87" s="35"/>
       <c r="V87" s="35"/>
@@ -12623,7 +12629,7 @@
       <c r="AI87" s="35"/>
       <c r="AJ87" s="35"/>
       <c r="AK87" s="35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AL87" s="35"/>
       <c r="AM87" s="35"/>
@@ -12666,7 +12672,7 @@
       <c r="R88" s="35"/>
       <c r="S88" s="35"/>
       <c r="T88" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="U88" s="35"/>
       <c r="V88" s="35"/>
@@ -12685,7 +12691,7 @@
       <c r="AI88" s="35"/>
       <c r="AJ88" s="35"/>
       <c r="AK88" s="35" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AL88" s="35"/>
       <c r="AM88" s="35"/>
@@ -13136,14 +13142,14 @@
     <mergeCell ref="AQ5:AS5"/>
     <mergeCell ref="F4:N4"/>
     <mergeCell ref="U4:AP4"/>
+    <mergeCell ref="L12:S13"/>
+    <mergeCell ref="T12:Y13"/>
+    <mergeCell ref="L15:AW16"/>
     <mergeCell ref="AX2:BE2"/>
     <mergeCell ref="AQ3:AW3"/>
     <mergeCell ref="AX3:BE3"/>
     <mergeCell ref="AT4:AW4"/>
     <mergeCell ref="BB4:BE4"/>
-    <mergeCell ref="L12:S13"/>
-    <mergeCell ref="T12:Y13"/>
-    <mergeCell ref="L15:AW16"/>
     <mergeCell ref="L9:N11"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="E2:AP3"/>

</xml_diff>

<commit_message>
ThaoNX/ThaoNX_Tuan4.docx: nop bao cao tuan 4
</commit_message>
<xml_diff>
--- a/Document/Design/SDD_GlobalConfiguration.xlsx
+++ b/Document/Design/SDD_GlobalConfiguration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="285" windowWidth="19020" windowHeight="8400" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="285" windowWidth="19020" windowHeight="8400" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -1544,7 +1544,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="185">
   <si>
     <t>&lt;Project Name&gt;</t>
   </si>
@@ -1897,9 +1897,6 @@
     <t>Thaonx</t>
   </si>
   <si>
-    <t>Media Option_Permission</t>
-  </si>
-  <si>
     <t>Configuration Site</t>
   </si>
   <si>
@@ -1909,9 +1906,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>Media Option_Component</t>
-  </si>
-  <si>
     <t>Create design for screen Configuration Site</t>
   </si>
   <si>
@@ -2066,6 +2060,45 @@
   </si>
   <si>
     <t xml:space="preserve">Welcome   </t>
+  </si>
+  <si>
+    <t>sitename</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>offlinemesage</t>
+  </si>
+  <si>
+    <t>editor</t>
+  </si>
+  <si>
+    <t>listlimit</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+  </si>
+  <si>
+    <t>varchar(200)</t>
+  </si>
+  <si>
+    <t>Add Item Definition  for screen Configuration Site</t>
+  </si>
+  <si>
+    <t>Add Item Definition  for screen Configuration System</t>
+  </si>
+  <si>
+    <t>Add Screen Prototype</t>
+  </si>
+  <si>
+    <t>Add Mapping screen items to Database</t>
+  </si>
+  <si>
+    <t>Add Events</t>
   </si>
 </sst>
 </file>
@@ -2765,7 +2798,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2997,6 +3030,9 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3031,9 +3067,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3081,6 +3114,7 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3438,8 +3472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G25"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3491,107 +3525,183 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="70">
-        <v>40705</v>
+        <v>40831</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>117</v>
       </c>
       <c r="D6" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="F6" s="8">
-        <v>0.1</v>
-      </c>
+      <c r="F6" s="8"/>
       <c r="G6" s="9" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="70">
-        <v>40706</v>
+        <v>40831</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D7" s="71" t="s">
-        <v>120</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0.1</v>
-      </c>
+      <c r="F7" s="8"/>
       <c r="G7" s="9" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="B8" s="121">
+        <v>40831</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="9"/>
+      <c r="G8" s="9" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="B9" s="121">
+        <v>40831</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>181</v>
+      </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
+      <c r="G9" s="9" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="B10" s="121">
+        <v>40832</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>182</v>
+      </c>
       <c r="F10" s="8"/>
-      <c r="G10" s="9"/>
+      <c r="G10" s="9" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="B11" s="121">
+        <v>40832</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>182</v>
+      </c>
       <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
+      <c r="G11" s="9" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="B12" s="121">
+        <v>40833</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>183</v>
+      </c>
       <c r="F12" s="8"/>
-      <c r="G12" s="9"/>
+      <c r="G12" s="9" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="B13" s="121">
+        <v>40833</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>183</v>
+      </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="9"/>
+      <c r="G13" s="9" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="B14" s="121">
+        <v>40835</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>184</v>
+      </c>
       <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
+      <c r="G14" s="9" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="B15" s="121">
+        <v>40835</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>184</v>
+      </c>
       <c r="F15" s="8"/>
-      <c r="G15" s="9"/>
+      <c r="G15" s="9" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="7"/>
@@ -3685,7 +3795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -3781,7 +3891,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="68" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4" s="21"/>
     </row>
@@ -3790,7 +3900,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="69" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" s="24"/>
     </row>
@@ -3944,8 +4054,8 @@
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C4" location="'Media Manager'!A1" display="Media Manager"/>
-    <hyperlink ref="C5" location="'Media Option_Permission'!A1" display="Media Option_Permission"/>
+    <hyperlink ref="C5" location="'Configuration System'!A1" display="Configuration System"/>
+    <hyperlink ref="C4" location="'Configuration Site'!A1" display="Configuration Site"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="96" orientation="portrait" r:id="rId1"/>
@@ -3956,9 +4066,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BE96"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AT6" sqref="AT6"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46:G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3971,51 +4081,51 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="104" t="s">
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="104"/>
-      <c r="K2" s="104"/>
-      <c r="L2" s="104"/>
-      <c r="M2" s="104"/>
-      <c r="N2" s="104"/>
-      <c r="O2" s="104"/>
-      <c r="P2" s="104"/>
-      <c r="Q2" s="104"/>
-      <c r="R2" s="104"/>
-      <c r="S2" s="104"/>
-      <c r="T2" s="104"/>
-      <c r="U2" s="104"/>
-      <c r="V2" s="104"/>
-      <c r="W2" s="104"/>
-      <c r="X2" s="104"/>
-      <c r="Y2" s="104"/>
-      <c r="Z2" s="104"/>
-      <c r="AA2" s="104"/>
-      <c r="AB2" s="104"/>
-      <c r="AC2" s="104"/>
-      <c r="AD2" s="104"/>
-      <c r="AE2" s="104"/>
-      <c r="AF2" s="104"/>
-      <c r="AG2" s="104"/>
-      <c r="AH2" s="104"/>
-      <c r="AI2" s="104"/>
-      <c r="AJ2" s="104"/>
-      <c r="AK2" s="104"/>
-      <c r="AL2" s="104"/>
-      <c r="AM2" s="104"/>
-      <c r="AN2" s="104"/>
-      <c r="AO2" s="104"/>
-      <c r="AP2" s="104"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="105"/>
+      <c r="S2" s="105"/>
+      <c r="T2" s="105"/>
+      <c r="U2" s="105"/>
+      <c r="V2" s="105"/>
+      <c r="W2" s="105"/>
+      <c r="X2" s="105"/>
+      <c r="Y2" s="105"/>
+      <c r="Z2" s="105"/>
+      <c r="AA2" s="105"/>
+      <c r="AB2" s="105"/>
+      <c r="AC2" s="105"/>
+      <c r="AD2" s="105"/>
+      <c r="AE2" s="105"/>
+      <c r="AF2" s="105"/>
+      <c r="AG2" s="105"/>
+      <c r="AH2" s="105"/>
+      <c r="AI2" s="105"/>
+      <c r="AJ2" s="105"/>
+      <c r="AK2" s="105"/>
+      <c r="AL2" s="105"/>
+      <c r="AM2" s="105"/>
+      <c r="AN2" s="105"/>
+      <c r="AO2" s="105"/>
+      <c r="AP2" s="105"/>
       <c r="AQ2" s="92" t="s">
         <v>7</v>
       </c>
@@ -4037,66 +4147,66 @@
       <c r="BE2" s="92"/>
     </row>
     <row r="3" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B3" s="103"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
-      <c r="P3" s="104"/>
-      <c r="Q3" s="104"/>
-      <c r="R3" s="104"/>
-      <c r="S3" s="104"/>
-      <c r="T3" s="104"/>
-      <c r="U3" s="104"/>
-      <c r="V3" s="104"/>
-      <c r="W3" s="104"/>
-      <c r="X3" s="104"/>
-      <c r="Y3" s="104"/>
-      <c r="Z3" s="104"/>
-      <c r="AA3" s="104"/>
-      <c r="AB3" s="104"/>
-      <c r="AC3" s="104"/>
-      <c r="AD3" s="104"/>
-      <c r="AE3" s="104"/>
-      <c r="AF3" s="104"/>
-      <c r="AG3" s="104"/>
-      <c r="AH3" s="104"/>
-      <c r="AI3" s="104"/>
-      <c r="AJ3" s="104"/>
-      <c r="AK3" s="104"/>
-      <c r="AL3" s="104"/>
-      <c r="AM3" s="104"/>
-      <c r="AN3" s="104"/>
-      <c r="AO3" s="104"/>
-      <c r="AP3" s="104"/>
-      <c r="AQ3" s="94" t="s">
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105"/>
+      <c r="M3" s="105"/>
+      <c r="N3" s="105"/>
+      <c r="O3" s="105"/>
+      <c r="P3" s="105"/>
+      <c r="Q3" s="105"/>
+      <c r="R3" s="105"/>
+      <c r="S3" s="105"/>
+      <c r="T3" s="105"/>
+      <c r="U3" s="105"/>
+      <c r="V3" s="105"/>
+      <c r="W3" s="105"/>
+      <c r="X3" s="105"/>
+      <c r="Y3" s="105"/>
+      <c r="Z3" s="105"/>
+      <c r="AA3" s="105"/>
+      <c r="AB3" s="105"/>
+      <c r="AC3" s="105"/>
+      <c r="AD3" s="105"/>
+      <c r="AE3" s="105"/>
+      <c r="AF3" s="105"/>
+      <c r="AG3" s="105"/>
+      <c r="AH3" s="105"/>
+      <c r="AI3" s="105"/>
+      <c r="AJ3" s="105"/>
+      <c r="AK3" s="105"/>
+      <c r="AL3" s="105"/>
+      <c r="AM3" s="105"/>
+      <c r="AN3" s="105"/>
+      <c r="AO3" s="105"/>
+      <c r="AP3" s="105"/>
+      <c r="AQ3" s="95" t="s">
         <v>108</v>
       </c>
-      <c r="AR3" s="94"/>
-      <c r="AS3" s="94"/>
-      <c r="AT3" s="94"/>
-      <c r="AU3" s="94"/>
-      <c r="AV3" s="94"/>
-      <c r="AW3" s="94"/>
-      <c r="AX3" s="95">
+      <c r="AR3" s="95"/>
+      <c r="AS3" s="95"/>
+      <c r="AT3" s="95"/>
+      <c r="AU3" s="95"/>
+      <c r="AV3" s="95"/>
+      <c r="AW3" s="95"/>
+      <c r="AX3" s="96">
         <v>40830</v>
       </c>
-      <c r="AY3" s="94"/>
-      <c r="AZ3" s="94"/>
-      <c r="BA3" s="94"/>
-      <c r="BB3" s="94"/>
-      <c r="BC3" s="94"/>
-      <c r="BD3" s="94"/>
-      <c r="BE3" s="94"/>
+      <c r="AY3" s="95"/>
+      <c r="AZ3" s="95"/>
+      <c r="BA3" s="95"/>
+      <c r="BB3" s="95"/>
+      <c r="BC3" s="95"/>
+      <c r="BD3" s="95"/>
+      <c r="BE3" s="95"/>
     </row>
     <row r="4" spans="2:57" x14ac:dyDescent="0.2">
       <c r="B4" s="106" t="s">
@@ -4105,140 +4215,140 @@
       <c r="C4" s="106"/>
       <c r="D4" s="106"/>
       <c r="E4" s="107"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="93"/>
-      <c r="J4" s="93"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="93"/>
-      <c r="M4" s="93"/>
-      <c r="N4" s="93"/>
-      <c r="O4" s="99" t="s">
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="102"/>
-      <c r="Q4" s="102"/>
-      <c r="R4" s="102"/>
-      <c r="S4" s="102"/>
-      <c r="T4" s="101"/>
-      <c r="U4" s="93" t="s">
+      <c r="P4" s="103"/>
+      <c r="Q4" s="103"/>
+      <c r="R4" s="103"/>
+      <c r="S4" s="103"/>
+      <c r="T4" s="102"/>
+      <c r="U4" s="94" t="s">
         <v>104</v>
       </c>
-      <c r="V4" s="93"/>
-      <c r="W4" s="93"/>
-      <c r="X4" s="93"/>
-      <c r="Y4" s="93"/>
-      <c r="Z4" s="93"/>
-      <c r="AA4" s="93"/>
-      <c r="AB4" s="93"/>
-      <c r="AC4" s="93"/>
-      <c r="AD4" s="93"/>
-      <c r="AE4" s="93"/>
-      <c r="AF4" s="93"/>
-      <c r="AG4" s="93"/>
-      <c r="AH4" s="93"/>
-      <c r="AI4" s="93"/>
-      <c r="AJ4" s="93"/>
-      <c r="AK4" s="93"/>
-      <c r="AL4" s="93"/>
-      <c r="AM4" s="93"/>
-      <c r="AN4" s="93"/>
-      <c r="AO4" s="93"/>
-      <c r="AP4" s="93"/>
-      <c r="AQ4" s="96" t="s">
+      <c r="V4" s="94"/>
+      <c r="W4" s="94"/>
+      <c r="X4" s="94"/>
+      <c r="Y4" s="94"/>
+      <c r="Z4" s="94"/>
+      <c r="AA4" s="94"/>
+      <c r="AB4" s="94"/>
+      <c r="AC4" s="94"/>
+      <c r="AD4" s="94"/>
+      <c r="AE4" s="94"/>
+      <c r="AF4" s="94"/>
+      <c r="AG4" s="94"/>
+      <c r="AH4" s="94"/>
+      <c r="AI4" s="94"/>
+      <c r="AJ4" s="94"/>
+      <c r="AK4" s="94"/>
+      <c r="AL4" s="94"/>
+      <c r="AM4" s="94"/>
+      <c r="AN4" s="94"/>
+      <c r="AO4" s="94"/>
+      <c r="AP4" s="94"/>
+      <c r="AQ4" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="AR4" s="97"/>
-      <c r="AS4" s="98"/>
-      <c r="AT4" s="105">
+      <c r="AR4" s="98"/>
+      <c r="AS4" s="99"/>
+      <c r="AT4" s="93">
         <v>40830</v>
       </c>
-      <c r="AU4" s="93"/>
-      <c r="AV4" s="93"/>
-      <c r="AW4" s="93"/>
-      <c r="AX4" s="96" t="s">
+      <c r="AU4" s="94"/>
+      <c r="AV4" s="94"/>
+      <c r="AW4" s="94"/>
+      <c r="AX4" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="AY4" s="97"/>
-      <c r="AZ4" s="97"/>
-      <c r="BA4" s="98"/>
-      <c r="BB4" s="105">
+      <c r="AY4" s="98"/>
+      <c r="AZ4" s="98"/>
+      <c r="BA4" s="99"/>
+      <c r="BB4" s="93">
         <v>40831</v>
       </c>
-      <c r="BC4" s="93"/>
-      <c r="BD4" s="93"/>
-      <c r="BE4" s="93"/>
+      <c r="BC4" s="94"/>
+      <c r="BD4" s="94"/>
+      <c r="BE4" s="94"/>
     </row>
     <row r="5" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="93"/>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93"/>
-      <c r="M5" s="93"/>
-      <c r="N5" s="93"/>
-      <c r="O5" s="99" t="s">
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="94"/>
+      <c r="L5" s="94"/>
+      <c r="M5" s="94"/>
+      <c r="N5" s="94"/>
+      <c r="O5" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="P5" s="102"/>
-      <c r="Q5" s="102"/>
-      <c r="R5" s="102"/>
-      <c r="S5" s="102"/>
-      <c r="T5" s="101"/>
-      <c r="U5" s="93"/>
-      <c r="V5" s="93"/>
-      <c r="W5" s="93"/>
-      <c r="X5" s="93"/>
-      <c r="Y5" s="93"/>
-      <c r="Z5" s="93"/>
-      <c r="AA5" s="93"/>
-      <c r="AB5" s="93"/>
-      <c r="AC5" s="93"/>
-      <c r="AD5" s="93"/>
-      <c r="AE5" s="93"/>
-      <c r="AF5" s="93"/>
-      <c r="AG5" s="93"/>
-      <c r="AH5" s="93"/>
-      <c r="AI5" s="93"/>
-      <c r="AJ5" s="93"/>
-      <c r="AK5" s="93"/>
-      <c r="AL5" s="93"/>
-      <c r="AM5" s="93"/>
-      <c r="AN5" s="93"/>
-      <c r="AO5" s="93"/>
-      <c r="AP5" s="93"/>
-      <c r="AQ5" s="99" t="s">
+      <c r="P5" s="103"/>
+      <c r="Q5" s="103"/>
+      <c r="R5" s="103"/>
+      <c r="S5" s="103"/>
+      <c r="T5" s="102"/>
+      <c r="U5" s="94"/>
+      <c r="V5" s="94"/>
+      <c r="W5" s="94"/>
+      <c r="X5" s="94"/>
+      <c r="Y5" s="94"/>
+      <c r="Z5" s="94"/>
+      <c r="AA5" s="94"/>
+      <c r="AB5" s="94"/>
+      <c r="AC5" s="94"/>
+      <c r="AD5" s="94"/>
+      <c r="AE5" s="94"/>
+      <c r="AF5" s="94"/>
+      <c r="AG5" s="94"/>
+      <c r="AH5" s="94"/>
+      <c r="AI5" s="94"/>
+      <c r="AJ5" s="94"/>
+      <c r="AK5" s="94"/>
+      <c r="AL5" s="94"/>
+      <c r="AM5" s="94"/>
+      <c r="AN5" s="94"/>
+      <c r="AO5" s="94"/>
+      <c r="AP5" s="94"/>
+      <c r="AQ5" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="AR5" s="100"/>
-      <c r="AS5" s="101"/>
-      <c r="AT5" s="105">
+      <c r="AR5" s="101"/>
+      <c r="AS5" s="102"/>
+      <c r="AT5" s="93">
         <v>40834</v>
       </c>
-      <c r="AU5" s="93"/>
-      <c r="AV5" s="93"/>
-      <c r="AW5" s="93"/>
-      <c r="AX5" s="99" t="s">
+      <c r="AU5" s="94"/>
+      <c r="AV5" s="94"/>
+      <c r="AW5" s="94"/>
+      <c r="AX5" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="AY5" s="102"/>
-      <c r="AZ5" s="102"/>
-      <c r="BA5" s="101"/>
-      <c r="BB5" s="105">
+      <c r="AY5" s="103"/>
+      <c r="AZ5" s="103"/>
+      <c r="BA5" s="102"/>
+      <c r="BB5" s="93">
         <v>40834</v>
       </c>
-      <c r="BC5" s="93"/>
-      <c r="BD5" s="93"/>
-      <c r="BE5" s="93"/>
+      <c r="BC5" s="94"/>
+      <c r="BD5" s="94"/>
+      <c r="BE5" s="94"/>
     </row>
     <row r="7" spans="2:57" x14ac:dyDescent="0.2">
       <c r="C7" s="108" t="s">
@@ -4466,7 +4576,7 @@
     </row>
     <row r="15" spans="2:57" x14ac:dyDescent="0.2">
       <c r="L15" s="83" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M15" s="84"/>
       <c r="N15" s="84"/>
@@ -4651,14 +4761,14 @@
       <c r="M20" s="41"/>
       <c r="N20" s="41"/>
       <c r="O20" s="41" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="P20" s="41"/>
       <c r="Q20" s="41"/>
       <c r="R20" s="41"/>
       <c r="S20" s="41"/>
       <c r="T20" s="73" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="U20" s="74"/>
       <c r="V20" s="74"/>
@@ -4735,14 +4845,14 @@
       <c r="M22" s="41"/>
       <c r="N22" s="41"/>
       <c r="O22" s="41" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="P22" s="41"/>
       <c r="Q22" s="41"/>
       <c r="R22" s="41"/>
       <c r="S22" s="41"/>
       <c r="T22" s="61" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="U22" s="62"/>
       <c r="V22" s="62"/>
@@ -4859,27 +4969,27 @@
       <c r="M25" s="41"/>
       <c r="N25" s="41"/>
       <c r="O25" s="41" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="P25" s="41"/>
       <c r="Q25" s="41"/>
       <c r="R25" s="41"/>
       <c r="S25" s="41"/>
       <c r="T25" s="76" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="U25" s="41" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="V25" s="41"/>
       <c r="W25" s="41"/>
       <c r="X25" s="41"/>
       <c r="Y25" s="41"/>
       <c r="Z25" s="76" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AA25" s="41" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AB25" s="41"/>
       <c r="AC25" s="41"/>
@@ -4949,14 +5059,14 @@
       <c r="M27" s="41"/>
       <c r="N27" s="41"/>
       <c r="O27" s="41" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="P27" s="41"/>
       <c r="Q27" s="41"/>
       <c r="R27" s="41"/>
       <c r="S27" s="41"/>
       <c r="T27" s="61" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="U27" s="62"/>
       <c r="V27" s="62"/>
@@ -5073,7 +5183,7 @@
       <c r="M30" s="41"/>
       <c r="N30" s="41"/>
       <c r="O30" s="41" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P30" s="41"/>
       <c r="Q30" s="41"/>
@@ -5082,7 +5192,7 @@
       <c r="T30" s="73"/>
       <c r="U30" s="74"/>
       <c r="V30" s="74" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="W30" s="74"/>
       <c r="X30" s="74"/>
@@ -5157,7 +5267,7 @@
       <c r="M32" s="41"/>
       <c r="N32" s="41"/>
       <c r="O32" s="41" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="P32" s="41"/>
       <c r="Q32" s="41"/>
@@ -5873,7 +5983,7 @@
       <c r="F54" s="35"/>
       <c r="G54" s="35"/>
       <c r="H54" s="35" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I54" s="35"/>
       <c r="J54" s="35"/>
@@ -5900,7 +6010,7 @@
       <c r="Y54" s="32"/>
       <c r="Z54" s="32"/>
       <c r="AA54" s="32" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="AB54" s="35"/>
       <c r="AC54" s="35"/>
@@ -5933,7 +6043,7 @@
       <c r="AV54" s="35"/>
       <c r="AW54" s="36"/>
       <c r="AX54" s="35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AY54" s="35"/>
       <c r="AZ54" s="35"/>
@@ -6128,7 +6238,7 @@
       <c r="Y57" s="32"/>
       <c r="Z57" s="32"/>
       <c r="AA57" s="32" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AB57" s="35"/>
       <c r="AC57" s="35"/>
@@ -6204,7 +6314,7 @@
       <c r="Y58" s="32"/>
       <c r="Z58" s="32"/>
       <c r="AA58" s="32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AB58" s="35"/>
       <c r="AC58" s="35"/>
@@ -6280,7 +6390,7 @@
       <c r="Y59" s="32"/>
       <c r="Z59" s="32"/>
       <c r="AA59" s="32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AB59" s="35"/>
       <c r="AC59" s="35"/>
@@ -6612,17 +6722,17 @@
       <c r="P66" s="31"/>
       <c r="Q66" s="34"/>
       <c r="R66" s="31"/>
-      <c r="S66" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="T66" s="31"/>
+      <c r="S66" s="31"/>
+      <c r="T66" s="33" t="s">
+        <v>53</v>
+      </c>
       <c r="U66" s="31"/>
       <c r="V66" s="31"/>
       <c r="W66" s="34"/>
       <c r="X66" s="31"/>
       <c r="Y66" s="31"/>
       <c r="Z66" s="33" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="AA66" s="31"/>
       <c r="AB66" s="31"/>
@@ -6631,7 +6741,7 @@
       <c r="AE66" s="31"/>
       <c r="AF66" s="31"/>
       <c r="AG66" s="31" t="s">
-        <v>53</v>
+        <v>172</v>
       </c>
       <c r="AH66" s="31"/>
       <c r="AI66" s="31"/>
@@ -6646,7 +6756,7 @@
       <c r="AR66" s="31"/>
       <c r="AS66" s="31"/>
       <c r="AT66" s="33" t="s">
-        <v>53</v>
+        <v>179</v>
       </c>
       <c r="AU66" s="31"/>
       <c r="AV66" s="31"/>
@@ -6678,17 +6788,17 @@
       <c r="P67" s="35"/>
       <c r="Q67" s="37"/>
       <c r="R67" s="35"/>
-      <c r="S67" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="T67" s="35"/>
+      <c r="S67" s="31"/>
+      <c r="T67" s="33" t="s">
+        <v>53</v>
+      </c>
       <c r="U67" s="35"/>
       <c r="V67" s="35"/>
       <c r="W67" s="37"/>
       <c r="X67" s="35"/>
       <c r="Y67" s="35"/>
       <c r="Z67" s="33" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="AA67" s="35"/>
       <c r="AB67" s="35"/>
@@ -6697,7 +6807,7 @@
       <c r="AE67" s="35"/>
       <c r="AF67" s="35"/>
       <c r="AG67" s="31" t="s">
-        <v>53</v>
+        <v>173</v>
       </c>
       <c r="AH67" s="35"/>
       <c r="AI67" s="35"/>
@@ -6712,7 +6822,7 @@
       <c r="AR67" s="35"/>
       <c r="AS67" s="35"/>
       <c r="AT67" s="33" t="s">
-        <v>53</v>
+        <v>177</v>
       </c>
       <c r="AU67" s="35"/>
       <c r="AV67" s="35"/>
@@ -6744,17 +6854,17 @@
       <c r="P68" s="35"/>
       <c r="Q68" s="37"/>
       <c r="R68" s="35"/>
-      <c r="S68" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="T68" s="35"/>
+      <c r="S68" s="31"/>
+      <c r="T68" s="33" t="s">
+        <v>53</v>
+      </c>
       <c r="U68" s="35"/>
       <c r="V68" s="35"/>
       <c r="W68" s="37"/>
       <c r="X68" s="35"/>
       <c r="Y68" s="35"/>
       <c r="Z68" s="33" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="AA68" s="35"/>
       <c r="AB68" s="35"/>
@@ -6763,7 +6873,7 @@
       <c r="AE68" s="35"/>
       <c r="AF68" s="35"/>
       <c r="AG68" s="31" t="s">
-        <v>53</v>
+        <v>174</v>
       </c>
       <c r="AH68" s="35"/>
       <c r="AI68" s="35"/>
@@ -6778,7 +6888,7 @@
       <c r="AR68" s="35"/>
       <c r="AS68" s="35"/>
       <c r="AT68" s="33" t="s">
-        <v>53</v>
+        <v>179</v>
       </c>
       <c r="AU68" s="35"/>
       <c r="AV68" s="35"/>
@@ -6810,17 +6920,17 @@
       <c r="P69" s="35"/>
       <c r="Q69" s="37"/>
       <c r="R69" s="35"/>
-      <c r="S69" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="T69" s="35"/>
+      <c r="S69" s="31"/>
+      <c r="T69" s="33" t="s">
+        <v>53</v>
+      </c>
       <c r="U69" s="35"/>
       <c r="V69" s="35"/>
       <c r="W69" s="37"/>
       <c r="X69" s="35"/>
       <c r="Y69" s="35"/>
       <c r="Z69" s="33" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="AA69" s="35"/>
       <c r="AB69" s="35"/>
@@ -6829,7 +6939,7 @@
       <c r="AE69" s="35"/>
       <c r="AF69" s="35"/>
       <c r="AG69" s="31" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="AH69" s="35"/>
       <c r="AI69" s="35"/>
@@ -6844,7 +6954,7 @@
       <c r="AR69" s="35"/>
       <c r="AS69" s="35"/>
       <c r="AT69" s="33" t="s">
-        <v>53</v>
+        <v>178</v>
       </c>
       <c r="AU69" s="35"/>
       <c r="AV69" s="35"/>
@@ -6876,17 +6986,17 @@
       <c r="P70" s="35"/>
       <c r="Q70" s="37"/>
       <c r="R70" s="35"/>
-      <c r="S70" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="T70" s="35"/>
+      <c r="S70" s="31"/>
+      <c r="T70" s="33" t="s">
+        <v>53</v>
+      </c>
       <c r="U70" s="35"/>
       <c r="V70" s="35"/>
       <c r="W70" s="37"/>
       <c r="X70" s="35"/>
       <c r="Y70" s="35"/>
       <c r="Z70" s="33" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="AA70" s="35"/>
       <c r="AB70" s="35"/>
@@ -6895,7 +7005,7 @@
       <c r="AE70" s="35"/>
       <c r="AF70" s="35"/>
       <c r="AG70" s="31" t="s">
-        <v>53</v>
+        <v>176</v>
       </c>
       <c r="AH70" s="35"/>
       <c r="AI70" s="35"/>
@@ -6910,7 +7020,7 @@
       <c r="AR70" s="35"/>
       <c r="AS70" s="35"/>
       <c r="AT70" s="33" t="s">
-        <v>53</v>
+        <v>177</v>
       </c>
       <c r="AU70" s="35"/>
       <c r="AV70" s="35"/>
@@ -7573,7 +7683,7 @@
       <c r="R85" s="31"/>
       <c r="S85" s="31"/>
       <c r="T85" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="U85" s="31"/>
       <c r="V85" s="31"/>
@@ -7591,7 +7701,7 @@
       <c r="AH85" s="31"/>
       <c r="AI85" s="31"/>
       <c r="AJ85" s="31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AK85" s="31"/>
       <c r="AL85" s="31"/>
@@ -7635,7 +7745,7 @@
       <c r="R86" s="35"/>
       <c r="S86" s="35"/>
       <c r="T86" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="U86" s="35"/>
       <c r="V86" s="35"/>
@@ -7653,7 +7763,7 @@
       <c r="AH86" s="35"/>
       <c r="AI86" s="35"/>
       <c r="AJ86" s="35" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AK86" s="35"/>
       <c r="AL86" s="35"/>
@@ -7697,7 +7807,7 @@
       <c r="R87" s="35"/>
       <c r="S87" s="35"/>
       <c r="T87" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="U87" s="35"/>
       <c r="V87" s="35"/>
@@ -7715,7 +7825,7 @@
       <c r="AH87" s="35"/>
       <c r="AI87" s="35"/>
       <c r="AJ87" s="35" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AK87" s="35"/>
       <c r="AL87" s="35"/>
@@ -7759,7 +7869,7 @@
       <c r="R88" s="35"/>
       <c r="S88" s="35"/>
       <c r="T88" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="U88" s="35"/>
       <c r="V88" s="35"/>
@@ -7777,7 +7887,7 @@
       <c r="AH88" s="35"/>
       <c r="AI88" s="35"/>
       <c r="AJ88" s="35" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AK88" s="35"/>
       <c r="AL88" s="35"/>
@@ -7821,7 +7931,7 @@
       <c r="R89" s="35"/>
       <c r="S89" s="35"/>
       <c r="T89" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="U89" s="35"/>
       <c r="V89" s="35"/>
@@ -7839,7 +7949,7 @@
       <c r="AH89" s="35"/>
       <c r="AI89" s="35"/>
       <c r="AJ89" s="35" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AK89" s="35"/>
       <c r="AL89" s="35"/>
@@ -8325,7 +8435,7 @@
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S65" sqref="S65"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8338,51 +8448,51 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="104" t="s">
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="104"/>
-      <c r="K2" s="104"/>
-      <c r="L2" s="104"/>
-      <c r="M2" s="104"/>
-      <c r="N2" s="104"/>
-      <c r="O2" s="104"/>
-      <c r="P2" s="104"/>
-      <c r="Q2" s="104"/>
-      <c r="R2" s="104"/>
-      <c r="S2" s="104"/>
-      <c r="T2" s="104"/>
-      <c r="U2" s="104"/>
-      <c r="V2" s="104"/>
-      <c r="W2" s="104"/>
-      <c r="X2" s="104"/>
-      <c r="Y2" s="104"/>
-      <c r="Z2" s="104"/>
-      <c r="AA2" s="104"/>
-      <c r="AB2" s="104"/>
-      <c r="AC2" s="104"/>
-      <c r="AD2" s="104"/>
-      <c r="AE2" s="104"/>
-      <c r="AF2" s="104"/>
-      <c r="AG2" s="104"/>
-      <c r="AH2" s="104"/>
-      <c r="AI2" s="104"/>
-      <c r="AJ2" s="104"/>
-      <c r="AK2" s="104"/>
-      <c r="AL2" s="104"/>
-      <c r="AM2" s="104"/>
-      <c r="AN2" s="104"/>
-      <c r="AO2" s="104"/>
-      <c r="AP2" s="104"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="105"/>
+      <c r="S2" s="105"/>
+      <c r="T2" s="105"/>
+      <c r="U2" s="105"/>
+      <c r="V2" s="105"/>
+      <c r="W2" s="105"/>
+      <c r="X2" s="105"/>
+      <c r="Y2" s="105"/>
+      <c r="Z2" s="105"/>
+      <c r="AA2" s="105"/>
+      <c r="AB2" s="105"/>
+      <c r="AC2" s="105"/>
+      <c r="AD2" s="105"/>
+      <c r="AE2" s="105"/>
+      <c r="AF2" s="105"/>
+      <c r="AG2" s="105"/>
+      <c r="AH2" s="105"/>
+      <c r="AI2" s="105"/>
+      <c r="AJ2" s="105"/>
+      <c r="AK2" s="105"/>
+      <c r="AL2" s="105"/>
+      <c r="AM2" s="105"/>
+      <c r="AN2" s="105"/>
+      <c r="AO2" s="105"/>
+      <c r="AP2" s="105"/>
       <c r="AQ2" s="92" t="s">
         <v>7</v>
       </c>
@@ -8404,66 +8514,66 @@
       <c r="BE2" s="92"/>
     </row>
     <row r="3" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B3" s="103"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
-      <c r="P3" s="104"/>
-      <c r="Q3" s="104"/>
-      <c r="R3" s="104"/>
-      <c r="S3" s="104"/>
-      <c r="T3" s="104"/>
-      <c r="U3" s="104"/>
-      <c r="V3" s="104"/>
-      <c r="W3" s="104"/>
-      <c r="X3" s="104"/>
-      <c r="Y3" s="104"/>
-      <c r="Z3" s="104"/>
-      <c r="AA3" s="104"/>
-      <c r="AB3" s="104"/>
-      <c r="AC3" s="104"/>
-      <c r="AD3" s="104"/>
-      <c r="AE3" s="104"/>
-      <c r="AF3" s="104"/>
-      <c r="AG3" s="104"/>
-      <c r="AH3" s="104"/>
-      <c r="AI3" s="104"/>
-      <c r="AJ3" s="104"/>
-      <c r="AK3" s="104"/>
-      <c r="AL3" s="104"/>
-      <c r="AM3" s="104"/>
-      <c r="AN3" s="104"/>
-      <c r="AO3" s="104"/>
-      <c r="AP3" s="104"/>
-      <c r="AQ3" s="94" t="s">
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105"/>
+      <c r="M3" s="105"/>
+      <c r="N3" s="105"/>
+      <c r="O3" s="105"/>
+      <c r="P3" s="105"/>
+      <c r="Q3" s="105"/>
+      <c r="R3" s="105"/>
+      <c r="S3" s="105"/>
+      <c r="T3" s="105"/>
+      <c r="U3" s="105"/>
+      <c r="V3" s="105"/>
+      <c r="W3" s="105"/>
+      <c r="X3" s="105"/>
+      <c r="Y3" s="105"/>
+      <c r="Z3" s="105"/>
+      <c r="AA3" s="105"/>
+      <c r="AB3" s="105"/>
+      <c r="AC3" s="105"/>
+      <c r="AD3" s="105"/>
+      <c r="AE3" s="105"/>
+      <c r="AF3" s="105"/>
+      <c r="AG3" s="105"/>
+      <c r="AH3" s="105"/>
+      <c r="AI3" s="105"/>
+      <c r="AJ3" s="105"/>
+      <c r="AK3" s="105"/>
+      <c r="AL3" s="105"/>
+      <c r="AM3" s="105"/>
+      <c r="AN3" s="105"/>
+      <c r="AO3" s="105"/>
+      <c r="AP3" s="105"/>
+      <c r="AQ3" s="95" t="s">
         <v>108</v>
       </c>
-      <c r="AR3" s="94"/>
-      <c r="AS3" s="94"/>
-      <c r="AT3" s="94"/>
-      <c r="AU3" s="94"/>
-      <c r="AV3" s="94"/>
-      <c r="AW3" s="94"/>
-      <c r="AX3" s="95">
+      <c r="AR3" s="95"/>
+      <c r="AS3" s="95"/>
+      <c r="AT3" s="95"/>
+      <c r="AU3" s="95"/>
+      <c r="AV3" s="95"/>
+      <c r="AW3" s="95"/>
+      <c r="AX3" s="96">
         <v>40830</v>
       </c>
-      <c r="AY3" s="94"/>
-      <c r="AZ3" s="94"/>
-      <c r="BA3" s="94"/>
-      <c r="BB3" s="94"/>
-      <c r="BC3" s="94"/>
-      <c r="BD3" s="94"/>
-      <c r="BE3" s="94"/>
+      <c r="AY3" s="95"/>
+      <c r="AZ3" s="95"/>
+      <c r="BA3" s="95"/>
+      <c r="BB3" s="95"/>
+      <c r="BC3" s="95"/>
+      <c r="BD3" s="95"/>
+      <c r="BE3" s="95"/>
     </row>
     <row r="4" spans="2:57" x14ac:dyDescent="0.2">
       <c r="B4" s="106" t="s">
@@ -8472,134 +8582,134 @@
       <c r="C4" s="106"/>
       <c r="D4" s="106"/>
       <c r="E4" s="107"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="93"/>
-      <c r="J4" s="93"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="93"/>
-      <c r="M4" s="93"/>
-      <c r="N4" s="93"/>
-      <c r="O4" s="99" t="s">
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="102"/>
-      <c r="Q4" s="102"/>
-      <c r="R4" s="102"/>
-      <c r="S4" s="102"/>
-      <c r="T4" s="101"/>
-      <c r="U4" s="93" t="s">
+      <c r="P4" s="103"/>
+      <c r="Q4" s="103"/>
+      <c r="R4" s="103"/>
+      <c r="S4" s="103"/>
+      <c r="T4" s="102"/>
+      <c r="U4" s="94" t="s">
         <v>104</v>
       </c>
-      <c r="V4" s="93"/>
-      <c r="W4" s="93"/>
-      <c r="X4" s="93"/>
-      <c r="Y4" s="93"/>
-      <c r="Z4" s="93"/>
-      <c r="AA4" s="93"/>
-      <c r="AB4" s="93"/>
-      <c r="AC4" s="93"/>
-      <c r="AD4" s="93"/>
-      <c r="AE4" s="93"/>
-      <c r="AF4" s="93"/>
-      <c r="AG4" s="93"/>
-      <c r="AH4" s="93"/>
-      <c r="AI4" s="93"/>
-      <c r="AJ4" s="93"/>
-      <c r="AK4" s="93"/>
-      <c r="AL4" s="93"/>
-      <c r="AM4" s="93"/>
-      <c r="AN4" s="93"/>
-      <c r="AO4" s="93"/>
-      <c r="AP4" s="93"/>
-      <c r="AQ4" s="96" t="s">
+      <c r="V4" s="94"/>
+      <c r="W4" s="94"/>
+      <c r="X4" s="94"/>
+      <c r="Y4" s="94"/>
+      <c r="Z4" s="94"/>
+      <c r="AA4" s="94"/>
+      <c r="AB4" s="94"/>
+      <c r="AC4" s="94"/>
+      <c r="AD4" s="94"/>
+      <c r="AE4" s="94"/>
+      <c r="AF4" s="94"/>
+      <c r="AG4" s="94"/>
+      <c r="AH4" s="94"/>
+      <c r="AI4" s="94"/>
+      <c r="AJ4" s="94"/>
+      <c r="AK4" s="94"/>
+      <c r="AL4" s="94"/>
+      <c r="AM4" s="94"/>
+      <c r="AN4" s="94"/>
+      <c r="AO4" s="94"/>
+      <c r="AP4" s="94"/>
+      <c r="AQ4" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="AR4" s="97"/>
-      <c r="AS4" s="98"/>
-      <c r="AT4" s="105">
+      <c r="AR4" s="98"/>
+      <c r="AS4" s="99"/>
+      <c r="AT4" s="93">
         <v>40830</v>
       </c>
-      <c r="AU4" s="93"/>
-      <c r="AV4" s="93"/>
-      <c r="AW4" s="93"/>
-      <c r="AX4" s="96" t="s">
+      <c r="AU4" s="94"/>
+      <c r="AV4" s="94"/>
+      <c r="AW4" s="94"/>
+      <c r="AX4" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="AY4" s="97"/>
-      <c r="AZ4" s="97"/>
-      <c r="BA4" s="98"/>
-      <c r="BB4" s="93"/>
-      <c r="BC4" s="93"/>
-      <c r="BD4" s="93"/>
-      <c r="BE4" s="93"/>
+      <c r="AY4" s="98"/>
+      <c r="AZ4" s="98"/>
+      <c r="BA4" s="99"/>
+      <c r="BB4" s="94"/>
+      <c r="BC4" s="94"/>
+      <c r="BD4" s="94"/>
+      <c r="BE4" s="94"/>
     </row>
     <row r="5" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="93"/>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93"/>
-      <c r="M5" s="93"/>
-      <c r="N5" s="93"/>
-      <c r="O5" s="99" t="s">
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="94"/>
+      <c r="L5" s="94"/>
+      <c r="M5" s="94"/>
+      <c r="N5" s="94"/>
+      <c r="O5" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="P5" s="102"/>
-      <c r="Q5" s="102"/>
-      <c r="R5" s="102"/>
-      <c r="S5" s="102"/>
-      <c r="T5" s="101"/>
-      <c r="U5" s="93"/>
-      <c r="V5" s="93"/>
-      <c r="W5" s="93"/>
-      <c r="X5" s="93"/>
-      <c r="Y5" s="93"/>
-      <c r="Z5" s="93"/>
-      <c r="AA5" s="93"/>
-      <c r="AB5" s="93"/>
-      <c r="AC5" s="93"/>
-      <c r="AD5" s="93"/>
-      <c r="AE5" s="93"/>
-      <c r="AF5" s="93"/>
-      <c r="AG5" s="93"/>
-      <c r="AH5" s="93"/>
-      <c r="AI5" s="93"/>
-      <c r="AJ5" s="93"/>
-      <c r="AK5" s="93"/>
-      <c r="AL5" s="93"/>
-      <c r="AM5" s="93"/>
-      <c r="AN5" s="93"/>
-      <c r="AO5" s="93"/>
-      <c r="AP5" s="93"/>
-      <c r="AQ5" s="99" t="s">
+      <c r="P5" s="103"/>
+      <c r="Q5" s="103"/>
+      <c r="R5" s="103"/>
+      <c r="S5" s="103"/>
+      <c r="T5" s="102"/>
+      <c r="U5" s="94"/>
+      <c r="V5" s="94"/>
+      <c r="W5" s="94"/>
+      <c r="X5" s="94"/>
+      <c r="Y5" s="94"/>
+      <c r="Z5" s="94"/>
+      <c r="AA5" s="94"/>
+      <c r="AB5" s="94"/>
+      <c r="AC5" s="94"/>
+      <c r="AD5" s="94"/>
+      <c r="AE5" s="94"/>
+      <c r="AF5" s="94"/>
+      <c r="AG5" s="94"/>
+      <c r="AH5" s="94"/>
+      <c r="AI5" s="94"/>
+      <c r="AJ5" s="94"/>
+      <c r="AK5" s="94"/>
+      <c r="AL5" s="94"/>
+      <c r="AM5" s="94"/>
+      <c r="AN5" s="94"/>
+      <c r="AO5" s="94"/>
+      <c r="AP5" s="94"/>
+      <c r="AQ5" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="AR5" s="100"/>
-      <c r="AS5" s="101"/>
-      <c r="AT5" s="93"/>
-      <c r="AU5" s="93"/>
-      <c r="AV5" s="93"/>
-      <c r="AW5" s="93"/>
-      <c r="AX5" s="99" t="s">
+      <c r="AR5" s="101"/>
+      <c r="AS5" s="102"/>
+      <c r="AT5" s="94"/>
+      <c r="AU5" s="94"/>
+      <c r="AV5" s="94"/>
+      <c r="AW5" s="94"/>
+      <c r="AX5" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="AY5" s="102"/>
-      <c r="AZ5" s="102"/>
-      <c r="BA5" s="101"/>
-      <c r="BB5" s="93"/>
-      <c r="BC5" s="93"/>
-      <c r="BD5" s="93"/>
-      <c r="BE5" s="93"/>
+      <c r="AY5" s="103"/>
+      <c r="AZ5" s="103"/>
+      <c r="BA5" s="102"/>
+      <c r="BB5" s="94"/>
+      <c r="BC5" s="94"/>
+      <c r="BD5" s="94"/>
+      <c r="BE5" s="94"/>
     </row>
     <row r="7" spans="2:57" x14ac:dyDescent="0.2">
       <c r="C7" s="108" t="s">
@@ -8827,7 +8937,7 @@
     </row>
     <row r="15" spans="2:57" x14ac:dyDescent="0.2">
       <c r="L15" s="83" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M15" s="84"/>
       <c r="N15" s="84"/>
@@ -8991,7 +9101,7 @@
       <c r="L19" s="44"/>
       <c r="M19" s="41"/>
       <c r="N19" s="41" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="O19" s="41"/>
       <c r="P19" s="41"/>
@@ -9001,7 +9111,7 @@
       <c r="T19" s="74"/>
       <c r="U19" s="74"/>
       <c r="V19" s="74" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="W19" s="74"/>
       <c r="X19" s="74"/>
@@ -9075,7 +9185,7 @@
       <c r="L21" s="44"/>
       <c r="M21" s="41"/>
       <c r="N21" s="41" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="O21" s="41"/>
       <c r="P21" s="41"/>
@@ -9085,7 +9195,7 @@
       <c r="T21" s="74"/>
       <c r="U21" s="74"/>
       <c r="V21" s="74" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="W21" s="74"/>
       <c r="X21" s="74"/>
@@ -9159,7 +9269,7 @@
       <c r="L23" s="44"/>
       <c r="M23" s="41"/>
       <c r="N23" s="41" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="O23" s="41"/>
       <c r="P23" s="41"/>
@@ -9169,7 +9279,7 @@
       <c r="T23" s="74"/>
       <c r="U23" s="74"/>
       <c r="V23" s="74" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="W23" s="74"/>
       <c r="X23" s="74"/>
@@ -9243,7 +9353,7 @@
       <c r="L25" s="44"/>
       <c r="M25" s="41"/>
       <c r="N25" s="41" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="O25" s="41"/>
       <c r="P25" s="41"/>
@@ -9253,7 +9363,7 @@
       <c r="T25" s="74"/>
       <c r="U25" s="74"/>
       <c r="V25" s="74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="W25" s="74"/>
       <c r="X25" s="74"/>
@@ -9327,7 +9437,7 @@
       <c r="L27" s="44"/>
       <c r="M27" s="41"/>
       <c r="N27" s="41" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="O27" s="41"/>
       <c r="P27" s="41"/>
@@ -9337,7 +9447,7 @@
       <c r="T27" s="74"/>
       <c r="U27" s="74"/>
       <c r="V27" s="74" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="W27" s="74"/>
       <c r="X27" s="74"/>
@@ -9451,24 +9561,24 @@
       <c r="L30" s="44"/>
       <c r="M30" s="41"/>
       <c r="N30" s="41" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="O30" s="41"/>
       <c r="P30" s="41"/>
       <c r="Q30" s="41"/>
       <c r="R30" s="41"/>
       <c r="S30" s="76" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T30" s="41" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="U30" s="41"/>
       <c r="V30" s="41"/>
       <c r="W30" s="41"/>
       <c r="X30" s="41"/>
       <c r="Y30" s="76" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Z30" s="41" t="s">
         <v>34</v>
@@ -9541,7 +9651,7 @@
       <c r="L32" s="44"/>
       <c r="M32" s="41"/>
       <c r="N32" s="41" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="O32" s="41"/>
       <c r="P32" s="41"/>
@@ -9551,7 +9661,7 @@
       <c r="T32" s="74"/>
       <c r="U32" s="74"/>
       <c r="V32" s="74" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="W32" s="74"/>
       <c r="X32" s="74"/>
@@ -9625,7 +9735,7 @@
       <c r="L34" s="44"/>
       <c r="M34" s="41"/>
       <c r="N34" s="41" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O34" s="41"/>
       <c r="P34" s="41"/>
@@ -9707,7 +9817,7 @@
       <c r="L36" s="44"/>
       <c r="M36" s="41"/>
       <c r="N36" s="41" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="O36" s="41"/>
       <c r="P36" s="41"/>
@@ -11426,7 +11536,7 @@
       <c r="Q65" s="34"/>
       <c r="R65" s="31"/>
       <c r="S65" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T65" s="31"/>
       <c r="U65" s="31"/>
@@ -11490,7 +11600,7 @@
       <c r="Q66" s="37"/>
       <c r="R66" s="35"/>
       <c r="S66" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T66" s="31"/>
       <c r="U66" s="31"/>
@@ -11554,7 +11664,7 @@
       <c r="Q67" s="37"/>
       <c r="R67" s="35"/>
       <c r="S67" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T67" s="31"/>
       <c r="U67" s="31"/>
@@ -11618,7 +11728,7 @@
       <c r="Q68" s="37"/>
       <c r="R68" s="35"/>
       <c r="S68" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T68" s="31"/>
       <c r="U68" s="31"/>
@@ -11682,7 +11792,7 @@
       <c r="Q69" s="37"/>
       <c r="R69" s="35"/>
       <c r="S69" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T69" s="31"/>
       <c r="U69" s="31"/>
@@ -11746,7 +11856,7 @@
       <c r="Q70" s="37"/>
       <c r="R70" s="35"/>
       <c r="S70" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T70" s="31"/>
       <c r="U70" s="31"/>
@@ -11810,7 +11920,7 @@
       <c r="Q71" s="37"/>
       <c r="R71" s="35"/>
       <c r="S71" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T71" s="31"/>
       <c r="U71" s="31"/>
@@ -11874,7 +11984,7 @@
       <c r="Q72" s="37"/>
       <c r="R72" s="35"/>
       <c r="S72" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T72" s="31"/>
       <c r="U72" s="31"/>
@@ -11938,7 +12048,7 @@
       <c r="Q73" s="37"/>
       <c r="R73" s="35"/>
       <c r="S73" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T73" s="31"/>
       <c r="U73" s="31"/>
@@ -12002,7 +12112,7 @@
       <c r="Q74" s="37"/>
       <c r="R74" s="35"/>
       <c r="S74" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T74" s="31"/>
       <c r="U74" s="31"/>
@@ -12066,7 +12176,7 @@
       <c r="Q75" s="37"/>
       <c r="R75" s="35"/>
       <c r="S75" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T75" s="31"/>
       <c r="U75" s="31"/>
@@ -12424,7 +12534,7 @@
       <c r="R84" s="31"/>
       <c r="S84" s="31"/>
       <c r="T84" s="31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="U84" s="31"/>
       <c r="V84" s="31"/>
@@ -12443,7 +12553,7 @@
       <c r="AI84" s="31"/>
       <c r="AJ84" s="31"/>
       <c r="AK84" s="31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AL84" s="31"/>
       <c r="AM84" s="31"/>
@@ -12486,7 +12596,7 @@
       <c r="R85" s="35"/>
       <c r="S85" s="35"/>
       <c r="T85" s="31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="U85" s="35"/>
       <c r="V85" s="35"/>
@@ -12505,7 +12615,7 @@
       <c r="AI85" s="35"/>
       <c r="AJ85" s="35"/>
       <c r="AK85" s="35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AL85" s="35"/>
       <c r="AM85" s="35"/>
@@ -12548,7 +12658,7 @@
       <c r="R86" s="35"/>
       <c r="S86" s="35"/>
       <c r="T86" s="31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="U86" s="35"/>
       <c r="V86" s="35"/>
@@ -12567,7 +12677,7 @@
       <c r="AI86" s="35"/>
       <c r="AJ86" s="35"/>
       <c r="AK86" s="35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AL86" s="35"/>
       <c r="AM86" s="35"/>
@@ -12610,7 +12720,7 @@
       <c r="R87" s="35"/>
       <c r="S87" s="35"/>
       <c r="T87" s="31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="U87" s="35"/>
       <c r="V87" s="35"/>
@@ -12629,7 +12739,7 @@
       <c r="AI87" s="35"/>
       <c r="AJ87" s="35"/>
       <c r="AK87" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AL87" s="35"/>
       <c r="AM87" s="35"/>
@@ -12672,7 +12782,7 @@
       <c r="R88" s="35"/>
       <c r="S88" s="35"/>
       <c r="T88" s="31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="U88" s="35"/>
       <c r="V88" s="35"/>
@@ -12691,7 +12801,7 @@
       <c r="AI88" s="35"/>
       <c r="AJ88" s="35"/>
       <c r="AK88" s="35" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AL88" s="35"/>
       <c r="AM88" s="35"/>

</xml_diff>